<commit_message>
set up data validation rules
</commit_message>
<xml_diff>
--- a/bio_info.xlsx
+++ b/bio_info.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isobe\fr\dragon-bios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACBBADC-22A1-45E5-8F01-1832937F3C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168C4D64-D69B-4529-B633-285C26FCB84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" state="hidden" r:id="rId1"/>
     <sheet name="dragons" sheetId="4" r:id="rId2"/>
-    <sheet name="Cumulative" sheetId="8" state="hidden" r:id="rId3"/>
+    <sheet name="validation" sheetId="9" r:id="rId3"/>
+    <sheet name="Cumulative" sheetId="8" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Flights">#REF!</definedName>
@@ -264,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="346">
   <si>
     <t>Dragon Info</t>
   </si>
@@ -1236,6 +1237,147 @@
   <si>
     <t>bio</t>
   </si>
+  <si>
+    <t>Straight alternative</t>
+  </si>
+  <si>
+    <t>flag</t>
+  </si>
+  <si>
+    <t>pronoun</t>
+  </si>
+  <si>
+    <t>Ammoth</t>
+  </si>
+  <si>
+    <t>MsB Grad</t>
+  </si>
+  <si>
+    <t>Diamond</t>
+  </si>
+  <si>
+    <t>Scrollwork</t>
+  </si>
+  <si>
+    <t>Wolfprints</t>
+  </si>
+  <si>
+    <t>Magdaneela</t>
+  </si>
+  <si>
+    <t>Lines</t>
+  </si>
+  <si>
+    <t>Aceflux</t>
+  </si>
+  <si>
+    <t>Aroace</t>
+  </si>
+  <si>
+    <t>Aroflux</t>
+  </si>
+  <si>
+    <t>Cisgender</t>
+  </si>
+  <si>
+    <t>Demiboy</t>
+  </si>
+  <si>
+    <t>Demiromantic</t>
+  </si>
+  <si>
+    <t>Gay man 7-stripe</t>
+  </si>
+  <si>
+    <t>Grey ace</t>
+  </si>
+  <si>
+    <t>Grey aro</t>
+  </si>
+  <si>
+    <t>Intersex</t>
+  </si>
+  <si>
+    <t>Non-SAM aromantic</t>
+  </si>
+  <si>
+    <t>Omnisexual</t>
+  </si>
+  <si>
+    <t>Oriented Aroace</t>
+  </si>
+  <si>
+    <t>Polysexual</t>
+  </si>
+  <si>
+    <t>Polyamorous</t>
+  </si>
+  <si>
+    <t>Queer Chevron</t>
+  </si>
+  <si>
+    <t>Queer Stripes</t>
+  </si>
+  <si>
+    <t>Quoisexual</t>
+  </si>
+  <si>
+    <t>Surgender</t>
+  </si>
+  <si>
+    <t>Transmasc</t>
+  </si>
+  <si>
+    <t>Pronoun Non-Conforming</t>
+  </si>
+  <si>
+    <t>Non-SAM asexual</t>
+  </si>
+  <si>
+    <t>Alloace</t>
+  </si>
+  <si>
+    <t>Bigender alternative</t>
+  </si>
+  <si>
+    <t>Rainbow 6-stripe</t>
+  </si>
+  <si>
+    <t>Rainbow 8-stripe</t>
+  </si>
+  <si>
+    <t>ey</t>
+  </si>
+  <si>
+    <t>fae</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>ze</t>
+  </si>
+  <si>
+    <t>Beastclans</t>
+  </si>
+  <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>Osiem</t>
+  </si>
+  <si>
+    <t>Decay</t>
+  </si>
+  <si>
+    <t>Books</t>
+  </si>
+  <si>
+    <t>Wooden</t>
+  </si>
+  <si>
+    <t>Scrolls L</t>
+  </si>
 </sst>
 </file>
 
@@ -1244,7 +1386,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yy"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1311,6 +1453,17 @@
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1662,7 +1815,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1759,6 +1912,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2166,31 +2323,31 @@
     </row>
     <row r="2" spans="1:23" ht="13.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="84"/>
+      <c r="C2" s="88"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="83" t="s">
+      <c r="H2" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="85"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="85"/>
-      <c r="U2" s="85"/>
-      <c r="V2" s="84"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="89"/>
+      <c r="P2" s="89"/>
+      <c r="Q2" s="89"/>
+      <c r="R2" s="89"/>
+      <c r="S2" s="89"/>
+      <c r="T2" s="89"/>
+      <c r="U2" s="89"/>
+      <c r="V2" s="88"/>
       <c r="W2" s="1"/>
     </row>
     <row r="3" spans="1:23" ht="13.2">
@@ -2205,21 +2362,21 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
-      <c r="Q3" s="87"/>
-      <c r="R3" s="87"/>
-      <c r="S3" s="87"/>
-      <c r="T3" s="87"/>
-      <c r="U3" s="87"/>
-      <c r="V3" s="88"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="91"/>
+      <c r="P3" s="91"/>
+      <c r="Q3" s="91"/>
+      <c r="R3" s="91"/>
+      <c r="S3" s="91"/>
+      <c r="T3" s="91"/>
+      <c r="U3" s="91"/>
+      <c r="V3" s="92"/>
       <c r="W3" s="1"/>
     </row>
     <row r="4" spans="1:23" ht="13.2">
@@ -2234,21 +2391,21 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="81"/>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="90"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="85"/>
+      <c r="Q4" s="85"/>
+      <c r="R4" s="85"/>
+      <c r="S4" s="85"/>
+      <c r="T4" s="85"/>
+      <c r="U4" s="85"/>
+      <c r="V4" s="94"/>
       <c r="W4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="13.2">
@@ -2269,21 +2426,21 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="81"/>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="90"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="85"/>
+      <c r="S5" s="85"/>
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="94"/>
       <c r="W5" s="1"/>
     </row>
     <row r="6" spans="1:23" ht="13.2">
@@ -2301,21 +2458,21 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="89"/>
-      <c r="I6" s="81"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="81"/>
-      <c r="L6" s="81"/>
-      <c r="M6" s="81"/>
-      <c r="N6" s="81"/>
-      <c r="O6" s="81"/>
-      <c r="P6" s="81"/>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="81"/>
-      <c r="T6" s="81"/>
-      <c r="U6" s="81"/>
-      <c r="V6" s="90"/>
+      <c r="H6" s="93"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="85"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="85"/>
+      <c r="O6" s="85"/>
+      <c r="P6" s="85"/>
+      <c r="Q6" s="85"/>
+      <c r="R6" s="85"/>
+      <c r="S6" s="85"/>
+      <c r="T6" s="85"/>
+      <c r="U6" s="85"/>
+      <c r="V6" s="94"/>
       <c r="W6" s="1"/>
     </row>
     <row r="7" spans="1:23" ht="13.2">
@@ -2330,21 +2487,21 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="91"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="92"/>
-      <c r="L7" s="92"/>
-      <c r="M7" s="92"/>
-      <c r="N7" s="92"/>
-      <c r="O7" s="92"/>
-      <c r="P7" s="92"/>
-      <c r="Q7" s="92"/>
-      <c r="R7" s="92"/>
-      <c r="S7" s="92"/>
-      <c r="T7" s="92"/>
-      <c r="U7" s="92"/>
-      <c r="V7" s="93"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="96"/>
+      <c r="K7" s="96"/>
+      <c r="L7" s="96"/>
+      <c r="M7" s="96"/>
+      <c r="N7" s="96"/>
+      <c r="O7" s="96"/>
+      <c r="P7" s="96"/>
+      <c r="Q7" s="96"/>
+      <c r="R7" s="96"/>
+      <c r="S7" s="96"/>
+      <c r="T7" s="96"/>
+      <c r="U7" s="96"/>
+      <c r="V7" s="97"/>
       <c r="W7" s="1"/>
     </row>
     <row r="8" spans="1:23" ht="13.2">
@@ -2374,26 +2531,26 @@
     </row>
     <row r="9" spans="1:23" ht="13.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="83" t="s">
+      <c r="B9" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="84"/>
+      <c r="C9" s="88"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="83" t="s">
+      <c r="H9" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="85"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="85"/>
-      <c r="M9" s="85"/>
-      <c r="N9" s="85"/>
-      <c r="O9" s="85"/>
-      <c r="P9" s="84"/>
-      <c r="Q9" s="82" t="str">
+      <c r="I9" s="89"/>
+      <c r="J9" s="89"/>
+      <c r="K9" s="89"/>
+      <c r="L9" s="89"/>
+      <c r="M9" s="89"/>
+      <c r="N9" s="89"/>
+      <c r="O9" s="89"/>
+      <c r="P9" s="88"/>
+      <c r="Q9" s="86" t="str">
         <f>IF(H11="","",CONCATENATE(IF(I10="","",CONCATENATE("
 [center][color=",$E$5,"][size=4]",I10,"[/size][/color][/center]
 ")),H11,"
@@ -2401,10 +2558,10 @@
         <v/>
       </c>
       <c r="R9" s="1"/>
-      <c r="S9" s="94" t="s">
+      <c r="S9" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="T9" s="88"/>
+      <c r="T9" s="92"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
@@ -2418,13 +2575,13 @@
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="80" t="str">
+      <c r="E10" s="84" t="str">
         <f>IF(NOT(C10=""),CONCATENATE("[center]",D12,"
 [size=2]",C10,"
 [i]",C11,"[/i][/size]"),"")</f>
         <v/>
       </c>
-      <c r="F10" s="82" t="str">
+      <c r="F10" s="86" t="str">
         <f>IF(AND(NOT(E16=""),NOT(D22="")),CONCATENATE("[columns][img]",#REF!,"[/img][nextcol]",E10,"[nextcol]",E13,E16,D22,"[/columns]"),IF(AND(NOT(E13=""),OR(AND(E16="",NOT(D22="")),AND(D22="",NOT(E16="")))),CONCATENATE("[columns][img]",#REF!,"[/img][nextcol]",E10,"[nextcol]",E13,E16,D22,"[/columns]"),IF(AND(NOT(E10=""),OR(AND(E13="",NOT(D22="")),AND(D22="",NOT(E13="")))),CONCATENATE("[columns][img]",#REF!,"[/img][nextcol]",E10,"[nextcol]",E13,D22,"[/columns]"),IF(AND(E13="",OR(AND(E10="",NOT(D22="")),AND(D22="",NOT(E10="")))),CONCATENATE(E10,D22,"[/center]"),""))))</f>
         <v/>
       </c>
@@ -2432,15 +2589,15 @@
       <c r="H10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="95"/>
-      <c r="J10" s="87"/>
-      <c r="K10" s="87"/>
-      <c r="L10" s="87"/>
-      <c r="M10" s="87"/>
-      <c r="N10" s="87"/>
-      <c r="O10" s="87"/>
-      <c r="P10" s="88"/>
-      <c r="Q10" s="81"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="91"/>
+      <c r="M10" s="91"/>
+      <c r="N10" s="91"/>
+      <c r="O10" s="91"/>
+      <c r="P10" s="92"/>
+      <c r="Q10" s="85"/>
       <c r="R10" s="1"/>
       <c r="S10" s="4" t="s">
         <v>17</v>
@@ -2459,19 +2616,19 @@
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
       <c r="G11" s="17"/>
-      <c r="H11" s="96"/>
-      <c r="I11" s="87"/>
-      <c r="J11" s="87"/>
-      <c r="K11" s="87"/>
-      <c r="L11" s="87"/>
-      <c r="M11" s="87"/>
-      <c r="N11" s="87"/>
-      <c r="O11" s="87"/>
-      <c r="P11" s="88"/>
-      <c r="Q11" s="81"/>
+      <c r="H11" s="100"/>
+      <c r="I11" s="91"/>
+      <c r="J11" s="91"/>
+      <c r="K11" s="91"/>
+      <c r="L11" s="91"/>
+      <c r="M11" s="91"/>
+      <c r="N11" s="91"/>
+      <c r="O11" s="91"/>
+      <c r="P11" s="92"/>
+      <c r="Q11" s="85"/>
       <c r="R11" s="1"/>
       <c r="S11" s="20"/>
       <c r="T11" s="21"/>
@@ -2480,7 +2637,7 @@
 [url=",T11,"][img]",S11,"[/img][/url]")))</f>
         <v/>
       </c>
-      <c r="V11" s="82" t="str">
+      <c r="V11" s="86" t="str">
         <f>IF(S11="","",CONCATENATE("
 [center][color=",E5,"][size=5]Art[/size][/color]
 [color=#000000][size=1]All pieces link to artist by click[/size][/color]
@@ -2490,7 +2647,7 @@
       </c>
       <c r="W11" s="17"/>
     </row>
-    <row r="12" spans="1:23" ht="15">
+    <row r="12" spans="1:23" ht="13.2">
       <c r="A12" s="1"/>
       <c r="B12" s="11" t="s">
         <v>20</v>
@@ -2500,19 +2657,19 @@
         <f>IF(NOT(C12=""),CONCATENATE("[url=http://flightrising.com/main.php?dragon=",C12,"][img]http://flightrising.com/rendern/portraits/",CEILING((C12+1)/100,1),"/",C12,"p.png[/img][/url]"),"")</f>
         <v/>
       </c>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
+      <c r="E12" s="85"/>
+      <c r="F12" s="85"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="89"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="81"/>
-      <c r="K12" s="81"/>
-      <c r="L12" s="81"/>
-      <c r="M12" s="81"/>
-      <c r="N12" s="81"/>
-      <c r="O12" s="81"/>
-      <c r="P12" s="90"/>
-      <c r="Q12" s="81"/>
+      <c r="H12" s="93"/>
+      <c r="I12" s="85"/>
+      <c r="J12" s="85"/>
+      <c r="K12" s="85"/>
+      <c r="L12" s="85"/>
+      <c r="M12" s="85"/>
+      <c r="N12" s="85"/>
+      <c r="O12" s="85"/>
+      <c r="P12" s="94"/>
+      <c r="Q12" s="85"/>
       <c r="R12" s="1"/>
       <c r="S12" s="25"/>
       <c r="T12" s="26"/>
@@ -2520,7 +2677,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V12" s="81"/>
+      <c r="V12" s="85"/>
       <c r="W12" s="1"/>
     </row>
     <row r="13" spans="1:23" ht="13.2">
@@ -2532,24 +2689,24 @@
       </c>
       <c r="C13" s="27"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="80" t="str">
+      <c r="E13" s="84" t="str">
         <f>IF(NOT(C13=""),CONCATENATE("[center]",D15,"
 [size=2]",C13,"
 [i]",C14,"[/i][/size][nextcol]"),"")</f>
         <v/>
       </c>
-      <c r="F13" s="81"/>
+      <c r="F13" s="85"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="89"/>
-      <c r="I13" s="81"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="81"/>
-      <c r="N13" s="81"/>
-      <c r="O13" s="81"/>
-      <c r="P13" s="90"/>
-      <c r="Q13" s="81"/>
+      <c r="H13" s="93"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="85"/>
+      <c r="L13" s="85"/>
+      <c r="M13" s="85"/>
+      <c r="N13" s="85"/>
+      <c r="O13" s="85"/>
+      <c r="P13" s="94"/>
+      <c r="Q13" s="85"/>
       <c r="R13" s="1"/>
       <c r="S13" s="28"/>
       <c r="T13" s="26"/>
@@ -2557,7 +2714,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V13" s="81"/>
+      <c r="V13" s="85"/>
       <c r="W13" s="1"/>
     </row>
     <row r="14" spans="1:23" ht="13.2">
@@ -2567,19 +2724,19 @@
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="81"/>
-      <c r="F14" s="81"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="89"/>
-      <c r="I14" s="81"/>
-      <c r="J14" s="81"/>
-      <c r="K14" s="81"/>
-      <c r="L14" s="81"/>
-      <c r="M14" s="81"/>
-      <c r="N14" s="81"/>
-      <c r="O14" s="81"/>
-      <c r="P14" s="90"/>
-      <c r="Q14" s="81"/>
+      <c r="H14" s="93"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="85"/>
+      <c r="L14" s="85"/>
+      <c r="M14" s="85"/>
+      <c r="N14" s="85"/>
+      <c r="O14" s="85"/>
+      <c r="P14" s="94"/>
+      <c r="Q14" s="85"/>
       <c r="R14" s="1"/>
       <c r="S14" s="28"/>
       <c r="T14" s="26"/>
@@ -2587,10 +2744,10 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V14" s="81"/>
+      <c r="V14" s="85"/>
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:23" ht="15">
+    <row r="15" spans="1:23" ht="13.2">
       <c r="A15" s="1"/>
       <c r="B15" s="6" t="s">
         <v>20</v>
@@ -2600,19 +2757,19 @@
         <f>IF(NOT(C15=""),CONCATENATE("[url=http://flightrising.com/main.php?dragon=",C15,"][img]http://flightrising.com/rendern/portraits/",CEILING((C15+1)/100,1),"/",C15,"p.png[/img][/url]"),"")</f>
         <v/>
       </c>
-      <c r="E15" s="81"/>
-      <c r="F15" s="81"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="85"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="91"/>
-      <c r="I15" s="92"/>
-      <c r="J15" s="92"/>
-      <c r="K15" s="92"/>
-      <c r="L15" s="92"/>
-      <c r="M15" s="92"/>
-      <c r="N15" s="92"/>
-      <c r="O15" s="92"/>
-      <c r="P15" s="93"/>
-      <c r="Q15" s="81"/>
+      <c r="H15" s="95"/>
+      <c r="I15" s="96"/>
+      <c r="J15" s="96"/>
+      <c r="K15" s="96"/>
+      <c r="L15" s="96"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="96"/>
+      <c r="O15" s="96"/>
+      <c r="P15" s="97"/>
+      <c r="Q15" s="85"/>
       <c r="R15" s="1"/>
       <c r="S15" s="25"/>
       <c r="T15" s="29"/>
@@ -2620,7 +2777,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V15" s="81"/>
+      <c r="V15" s="85"/>
       <c r="W15" s="1"/>
     </row>
     <row r="16" spans="1:23" ht="13.2">
@@ -2632,13 +2789,13 @@
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="80" t="str">
+      <c r="E16" s="84" t="str">
         <f>IF(NOT(C16=""),CONCATENATE("[center]",D18,"
 [size=2]",C16,"
 [i]",C17,"[/i][/size][nextcol]"),"")</f>
         <v/>
       </c>
-      <c r="F16" s="81"/>
+      <c r="F16" s="85"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -2657,7 +2814,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V16" s="81"/>
+      <c r="V16" s="85"/>
       <c r="W16" s="1"/>
     </row>
     <row r="17" spans="1:23" ht="13.2">
@@ -2667,21 +2824,21 @@
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="81"/>
-      <c r="F17" s="81"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="85"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="83" t="s">
+      <c r="H17" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="85"/>
-      <c r="J17" s="85"/>
-      <c r="K17" s="85"/>
-      <c r="L17" s="85"/>
-      <c r="M17" s="85"/>
-      <c r="N17" s="85"/>
-      <c r="O17" s="85"/>
-      <c r="P17" s="84"/>
-      <c r="Q17" s="82" t="str">
+      <c r="I17" s="89"/>
+      <c r="J17" s="89"/>
+      <c r="K17" s="89"/>
+      <c r="L17" s="89"/>
+      <c r="M17" s="89"/>
+      <c r="N17" s="89"/>
+      <c r="O17" s="89"/>
+      <c r="P17" s="88"/>
+      <c r="Q17" s="86" t="str">
         <f>IF(H19="","",CONCATENATE(IF(I18="","",CONCATENATE("
 [center][color=",$E$5,"][size=4]",I18,"[/size][/color][/center]
 ")),"
@@ -2696,10 +2853,10 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V17" s="81"/>
+      <c r="V17" s="85"/>
       <c r="W17" s="1"/>
     </row>
-    <row r="18" spans="1:23" ht="15">
+    <row r="18" spans="1:23" ht="13.2">
       <c r="A18" s="1"/>
       <c r="B18" s="11" t="s">
         <v>20</v>
@@ -2709,21 +2866,21 @@
         <f>IF(NOT(C18=""),CONCATENATE("[url=http://flightrising.com/main.php?dragon=",C18,"][img]http://flightrising.com/rendern/portraits/",CEILING((C18+1)/100,1),"/",C18,"p.png[/img][/url]"),"")</f>
         <v/>
       </c>
-      <c r="E18" s="81"/>
-      <c r="F18" s="81"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="85"/>
       <c r="G18" s="1"/>
       <c r="H18" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="95"/>
-      <c r="J18" s="87"/>
-      <c r="K18" s="87"/>
-      <c r="L18" s="87"/>
-      <c r="M18" s="87"/>
-      <c r="N18" s="87"/>
-      <c r="O18" s="87"/>
-      <c r="P18" s="88"/>
-      <c r="Q18" s="81"/>
+      <c r="I18" s="99"/>
+      <c r="J18" s="91"/>
+      <c r="K18" s="91"/>
+      <c r="L18" s="91"/>
+      <c r="M18" s="91"/>
+      <c r="N18" s="91"/>
+      <c r="O18" s="91"/>
+      <c r="P18" s="92"/>
+      <c r="Q18" s="85"/>
       <c r="R18" s="1"/>
       <c r="S18" s="28"/>
       <c r="T18" s="26"/>
@@ -2731,7 +2888,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V18" s="81"/>
+      <c r="V18" s="85"/>
       <c r="W18" s="1"/>
     </row>
     <row r="19" spans="1:23" ht="13.2">
@@ -2742,16 +2899,16 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="96"/>
-      <c r="I19" s="87"/>
-      <c r="J19" s="87"/>
-      <c r="K19" s="87"/>
-      <c r="L19" s="87"/>
-      <c r="M19" s="87"/>
-      <c r="N19" s="87"/>
-      <c r="O19" s="87"/>
-      <c r="P19" s="88"/>
-      <c r="Q19" s="81"/>
+      <c r="H19" s="100"/>
+      <c r="I19" s="91"/>
+      <c r="J19" s="91"/>
+      <c r="K19" s="91"/>
+      <c r="L19" s="91"/>
+      <c r="M19" s="91"/>
+      <c r="N19" s="91"/>
+      <c r="O19" s="91"/>
+      <c r="P19" s="92"/>
+      <c r="Q19" s="85"/>
       <c r="R19" s="1"/>
       <c r="S19" s="28"/>
       <c r="T19" s="26"/>
@@ -2759,29 +2916,29 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V19" s="81"/>
+      <c r="V19" s="85"/>
       <c r="W19" s="1"/>
     </row>
     <row r="20" spans="1:23" ht="13.2">
       <c r="A20" s="1"/>
-      <c r="B20" s="83" t="s">
+      <c r="B20" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="84"/>
+      <c r="C20" s="88"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="89"/>
-      <c r="I20" s="81"/>
-      <c r="J20" s="81"/>
-      <c r="K20" s="81"/>
-      <c r="L20" s="81"/>
-      <c r="M20" s="81"/>
-      <c r="N20" s="81"/>
-      <c r="O20" s="81"/>
-      <c r="P20" s="90"/>
-      <c r="Q20" s="81"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="85"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="85"/>
+      <c r="L20" s="85"/>
+      <c r="M20" s="85"/>
+      <c r="N20" s="85"/>
+      <c r="O20" s="85"/>
+      <c r="P20" s="94"/>
+      <c r="Q20" s="85"/>
       <c r="R20" s="1"/>
       <c r="S20" s="28"/>
       <c r="T20" s="26"/>
@@ -2789,7 +2946,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V20" s="81"/>
+      <c r="V20" s="85"/>
       <c r="W20" s="1"/>
     </row>
     <row r="21" spans="1:23" ht="13.2">
@@ -2805,16 +2962,16 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="89"/>
-      <c r="I21" s="81"/>
-      <c r="J21" s="81"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="81"/>
-      <c r="M21" s="81"/>
-      <c r="N21" s="81"/>
-      <c r="O21" s="81"/>
-      <c r="P21" s="90"/>
-      <c r="Q21" s="81"/>
+      <c r="H21" s="93"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="85"/>
+      <c r="K21" s="85"/>
+      <c r="L21" s="85"/>
+      <c r="M21" s="85"/>
+      <c r="N21" s="85"/>
+      <c r="O21" s="85"/>
+      <c r="P21" s="94"/>
+      <c r="Q21" s="85"/>
       <c r="R21" s="1"/>
       <c r="S21" s="28"/>
       <c r="T21" s="26"/>
@@ -2822,10 +2979,10 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V21" s="81"/>
+      <c r="V21" s="85"/>
       <c r="W21" s="1"/>
     </row>
-    <row r="22" spans="1:23" ht="15">
+    <row r="22" spans="1:23" ht="13.2">
       <c r="A22" s="1"/>
       <c r="B22" s="31" t="s">
         <v>2</v>
@@ -2839,16 +2996,16 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="89"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="81"/>
-      <c r="O22" s="81"/>
-      <c r="P22" s="90"/>
-      <c r="Q22" s="81"/>
+      <c r="H22" s="93"/>
+      <c r="I22" s="85"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="85"/>
+      <c r="L22" s="85"/>
+      <c r="M22" s="85"/>
+      <c r="N22" s="85"/>
+      <c r="O22" s="85"/>
+      <c r="P22" s="94"/>
+      <c r="Q22" s="85"/>
       <c r="R22" s="1"/>
       <c r="S22" s="28"/>
       <c r="T22" s="26"/>
@@ -2856,7 +3013,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V22" s="81"/>
+      <c r="V22" s="85"/>
       <c r="W22" s="1"/>
     </row>
     <row r="23" spans="1:23" ht="13.2">
@@ -2867,16 +3024,16 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="91"/>
-      <c r="I23" s="92"/>
-      <c r="J23" s="92"/>
-      <c r="K23" s="92"/>
-      <c r="L23" s="92"/>
-      <c r="M23" s="92"/>
-      <c r="N23" s="92"/>
-      <c r="O23" s="92"/>
-      <c r="P23" s="93"/>
-      <c r="Q23" s="81"/>
+      <c r="H23" s="95"/>
+      <c r="I23" s="96"/>
+      <c r="J23" s="96"/>
+      <c r="K23" s="96"/>
+      <c r="L23" s="96"/>
+      <c r="M23" s="96"/>
+      <c r="N23" s="96"/>
+      <c r="O23" s="96"/>
+      <c r="P23" s="97"/>
+      <c r="Q23" s="85"/>
       <c r="R23" s="1"/>
       <c r="S23" s="28"/>
       <c r="T23" s="26"/>
@@ -2884,15 +3041,15 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V23" s="81"/>
+      <c r="V23" s="85"/>
       <c r="W23" s="1"/>
     </row>
     <row r="24" spans="1:23" ht="13.2">
       <c r="A24" s="1"/>
-      <c r="B24" s="83" t="s">
+      <c r="B24" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="84"/>
+      <c r="C24" s="88"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -2914,7 +3071,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V24" s="81"/>
+      <c r="V24" s="85"/>
       <c r="W24" s="1"/>
     </row>
     <row r="25" spans="1:23" ht="13.2">
@@ -2931,17 +3088,17 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="83" t="s">
+      <c r="H25" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="85"/>
-      <c r="J25" s="85"/>
-      <c r="K25" s="85"/>
-      <c r="L25" s="85"/>
-      <c r="M25" s="85"/>
-      <c r="N25" s="85"/>
-      <c r="O25" s="85"/>
-      <c r="P25" s="84"/>
+      <c r="I25" s="89"/>
+      <c r="J25" s="89"/>
+      <c r="K25" s="89"/>
+      <c r="L25" s="89"/>
+      <c r="M25" s="89"/>
+      <c r="N25" s="89"/>
+      <c r="O25" s="89"/>
+      <c r="P25" s="88"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="34"/>
@@ -2950,7 +3107,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V25" s="81"/>
+      <c r="V25" s="85"/>
       <c r="W25" s="1"/>
     </row>
     <row r="26" spans="1:23" ht="13.2">
@@ -2989,11 +3146,11 @@
         <f>CONCATENATE(M26,M28,"[br]",M27,M29,"[br][img]https://i.imgur.com/4bD1JYI.png[/img]")</f>
         <v>#REF!</v>
       </c>
-      <c r="O26" s="98" t="e">
+      <c r="O26" s="102" t="e">
         <f ca="1">image(L26,3)</f>
         <v>#NAME?</v>
       </c>
-      <c r="P26" s="99" t="e">
+      <c r="P26" s="103" t="e">
         <f ca="1">image(L28,3)</f>
         <v>#NAME?</v>
       </c>
@@ -3037,24 +3194,24 @@
         <v/>
       </c>
       <c r="N27" s="43"/>
-      <c r="O27" s="89"/>
-      <c r="P27" s="90"/>
+      <c r="O27" s="93"/>
+      <c r="P27" s="94"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
-      <c r="S27" s="83" t="s">
+      <c r="S27" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="T27" s="84"/>
+      <c r="T27" s="88"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
     </row>
     <row r="28" spans="1:23" ht="13.2">
       <c r="A28" s="1"/>
-      <c r="B28" s="83" t="s">
+      <c r="B28" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="84"/>
+      <c r="C28" s="88"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -3078,11 +3235,11 @@
         <v>#REF!</v>
       </c>
       <c r="N28" s="43"/>
-      <c r="O28" s="100" t="e">
+      <c r="O28" s="104" t="e">
         <f ca="1">image(L27,3)</f>
         <v>#NAME?</v>
       </c>
-      <c r="P28" s="101" t="e">
+      <c r="P28" s="105" t="e">
         <f ca="1">image(L29,3)</f>
         <v>#NAME?</v>
       </c>
@@ -3094,13 +3251,13 @@
       <c r="T28" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="U28" s="82" t="e">
+      <c r="U28" s="86" t="e">
         <f>IF(OR(T28="",T28="No"),"",CONCATENATE("[center][img]http://i.imgur.com/fnF3LPe.png[/img][/center]
 ",IF(OR(T29="",T29=1),"",CONCATENATE("[center][size=2]",T29," time winner[/size][/center]
 ")),D5))</f>
         <v>#REF!</v>
       </c>
-      <c r="V28" s="81"/>
+      <c r="V28" s="85"/>
       <c r="W28" s="1"/>
     </row>
     <row r="29" spans="1:23" ht="13.2">
@@ -3132,16 +3289,16 @@
         <v>#REF!</v>
       </c>
       <c r="N29" s="47"/>
-      <c r="O29" s="91"/>
-      <c r="P29" s="93"/>
+      <c r="O29" s="95"/>
+      <c r="P29" s="97"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="11" t="s">
         <v>44</v>
       </c>
       <c r="T29" s="23"/>
-      <c r="U29" s="81"/>
-      <c r="V29" s="81"/>
+      <c r="U29" s="85"/>
+      <c r="V29" s="85"/>
       <c r="W29" s="1"/>
     </row>
     <row r="30" spans="1:23" ht="13.2">
@@ -3171,34 +3328,34 @@
     </row>
     <row r="31" spans="1:23" ht="13.2">
       <c r="A31" s="1"/>
-      <c r="B31" s="83" t="s">
+      <c r="B31" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="85"/>
-      <c r="D31" s="85"/>
-      <c r="E31" s="85"/>
-      <c r="F31" s="85"/>
-      <c r="G31" s="85"/>
-      <c r="H31" s="85"/>
-      <c r="I31" s="85"/>
-      <c r="J31" s="85"/>
-      <c r="K31" s="85"/>
-      <c r="L31" s="85"/>
-      <c r="M31" s="85"/>
-      <c r="N31" s="85"/>
-      <c r="O31" s="85"/>
-      <c r="P31" s="85"/>
-      <c r="Q31" s="85"/>
-      <c r="R31" s="85"/>
-      <c r="S31" s="85"/>
-      <c r="T31" s="85"/>
-      <c r="U31" s="85"/>
-      <c r="V31" s="84"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="89"/>
+      <c r="G31" s="89"/>
+      <c r="H31" s="89"/>
+      <c r="I31" s="89"/>
+      <c r="J31" s="89"/>
+      <c r="K31" s="89"/>
+      <c r="L31" s="89"/>
+      <c r="M31" s="89"/>
+      <c r="N31" s="89"/>
+      <c r="O31" s="89"/>
+      <c r="P31" s="89"/>
+      <c r="Q31" s="89"/>
+      <c r="R31" s="89"/>
+      <c r="S31" s="89"/>
+      <c r="T31" s="89"/>
+      <c r="U31" s="89"/>
+      <c r="V31" s="88"/>
       <c r="W31" s="1"/>
     </row>
     <row r="32" spans="1:23" ht="13.2">
       <c r="A32" s="1"/>
-      <c r="B32" s="97" t="e">
+      <c r="B32" s="101" t="e">
         <f>CONCATENATE(IF(N26="",CONCATENATE("[center][color=",E5,"][size=6]",UPPER(C3),"[/size]
 [size=4]",C4,"[/size][/color]
 ",D5,"[/center]"),CONCATENATE("[columns][img]https://i.imgur.com/4bD1JYI.png[/img][nextcol][center][color=",E5,"][size=6]",C3,"[/size]
@@ -3217,401 +3374,401 @@
 Pride icons: Boneless 78150","")),"[/size][/right]")</f>
         <v>#REF!</v>
       </c>
-      <c r="C32" s="87"/>
-      <c r="D32" s="87"/>
-      <c r="E32" s="87"/>
-      <c r="F32" s="87"/>
-      <c r="G32" s="87"/>
-      <c r="H32" s="87"/>
-      <c r="I32" s="87"/>
-      <c r="J32" s="87"/>
-      <c r="K32" s="87"/>
-      <c r="L32" s="87"/>
-      <c r="M32" s="87"/>
-      <c r="N32" s="87"/>
-      <c r="O32" s="87"/>
-      <c r="P32" s="87"/>
-      <c r="Q32" s="87"/>
-      <c r="R32" s="87"/>
-      <c r="S32" s="87"/>
-      <c r="T32" s="87"/>
-      <c r="U32" s="87"/>
-      <c r="V32" s="88"/>
+      <c r="C32" s="91"/>
+      <c r="D32" s="91"/>
+      <c r="E32" s="91"/>
+      <c r="F32" s="91"/>
+      <c r="G32" s="91"/>
+      <c r="H32" s="91"/>
+      <c r="I32" s="91"/>
+      <c r="J32" s="91"/>
+      <c r="K32" s="91"/>
+      <c r="L32" s="91"/>
+      <c r="M32" s="91"/>
+      <c r="N32" s="91"/>
+      <c r="O32" s="91"/>
+      <c r="P32" s="91"/>
+      <c r="Q32" s="91"/>
+      <c r="R32" s="91"/>
+      <c r="S32" s="91"/>
+      <c r="T32" s="91"/>
+      <c r="U32" s="91"/>
+      <c r="V32" s="92"/>
       <c r="W32" s="1"/>
     </row>
     <row r="33" spans="1:23" ht="13.2">
       <c r="A33" s="1"/>
-      <c r="B33" s="89"/>
-      <c r="C33" s="81"/>
-      <c r="D33" s="81"/>
-      <c r="E33" s="81"/>
-      <c r="F33" s="81"/>
-      <c r="G33" s="81"/>
-      <c r="H33" s="81"/>
-      <c r="I33" s="81"/>
-      <c r="J33" s="81"/>
-      <c r="K33" s="81"/>
-      <c r="L33" s="81"/>
-      <c r="M33" s="81"/>
-      <c r="N33" s="81"/>
-      <c r="O33" s="81"/>
-      <c r="P33" s="81"/>
-      <c r="Q33" s="81"/>
-      <c r="R33" s="81"/>
-      <c r="S33" s="81"/>
-      <c r="T33" s="81"/>
-      <c r="U33" s="81"/>
-      <c r="V33" s="90"/>
+      <c r="B33" s="93"/>
+      <c r="C33" s="85"/>
+      <c r="D33" s="85"/>
+      <c r="E33" s="85"/>
+      <c r="F33" s="85"/>
+      <c r="G33" s="85"/>
+      <c r="H33" s="85"/>
+      <c r="I33" s="85"/>
+      <c r="J33" s="85"/>
+      <c r="K33" s="85"/>
+      <c r="L33" s="85"/>
+      <c r="M33" s="85"/>
+      <c r="N33" s="85"/>
+      <c r="O33" s="85"/>
+      <c r="P33" s="85"/>
+      <c r="Q33" s="85"/>
+      <c r="R33" s="85"/>
+      <c r="S33" s="85"/>
+      <c r="T33" s="85"/>
+      <c r="U33" s="85"/>
+      <c r="V33" s="94"/>
       <c r="W33" s="1"/>
     </row>
     <row r="34" spans="1:23" ht="13.2">
       <c r="A34" s="1"/>
-      <c r="B34" s="89"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="81"/>
-      <c r="G34" s="81"/>
-      <c r="H34" s="81"/>
-      <c r="I34" s="81"/>
-      <c r="J34" s="81"/>
-      <c r="K34" s="81"/>
-      <c r="L34" s="81"/>
-      <c r="M34" s="81"/>
-      <c r="N34" s="81"/>
-      <c r="O34" s="81"/>
-      <c r="P34" s="81"/>
-      <c r="Q34" s="81"/>
-      <c r="R34" s="81"/>
-      <c r="S34" s="81"/>
-      <c r="T34" s="81"/>
-      <c r="U34" s="81"/>
-      <c r="V34" s="90"/>
+      <c r="B34" s="93"/>
+      <c r="C34" s="85"/>
+      <c r="D34" s="85"/>
+      <c r="E34" s="85"/>
+      <c r="F34" s="85"/>
+      <c r="G34" s="85"/>
+      <c r="H34" s="85"/>
+      <c r="I34" s="85"/>
+      <c r="J34" s="85"/>
+      <c r="K34" s="85"/>
+      <c r="L34" s="85"/>
+      <c r="M34" s="85"/>
+      <c r="N34" s="85"/>
+      <c r="O34" s="85"/>
+      <c r="P34" s="85"/>
+      <c r="Q34" s="85"/>
+      <c r="R34" s="85"/>
+      <c r="S34" s="85"/>
+      <c r="T34" s="85"/>
+      <c r="U34" s="85"/>
+      <c r="V34" s="94"/>
       <c r="W34" s="1"/>
     </row>
     <row r="35" spans="1:23" ht="13.2">
       <c r="A35" s="1"/>
-      <c r="B35" s="89"/>
-      <c r="C35" s="81"/>
-      <c r="D35" s="81"/>
-      <c r="E35" s="81"/>
-      <c r="F35" s="81"/>
-      <c r="G35" s="81"/>
-      <c r="H35" s="81"/>
-      <c r="I35" s="81"/>
-      <c r="J35" s="81"/>
-      <c r="K35" s="81"/>
-      <c r="L35" s="81"/>
-      <c r="M35" s="81"/>
-      <c r="N35" s="81"/>
-      <c r="O35" s="81"/>
-      <c r="P35" s="81"/>
-      <c r="Q35" s="81"/>
-      <c r="R35" s="81"/>
-      <c r="S35" s="81"/>
-      <c r="T35" s="81"/>
-      <c r="U35" s="81"/>
-      <c r="V35" s="90"/>
+      <c r="B35" s="93"/>
+      <c r="C35" s="85"/>
+      <c r="D35" s="85"/>
+      <c r="E35" s="85"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="85"/>
+      <c r="H35" s="85"/>
+      <c r="I35" s="85"/>
+      <c r="J35" s="85"/>
+      <c r="K35" s="85"/>
+      <c r="L35" s="85"/>
+      <c r="M35" s="85"/>
+      <c r="N35" s="85"/>
+      <c r="O35" s="85"/>
+      <c r="P35" s="85"/>
+      <c r="Q35" s="85"/>
+      <c r="R35" s="85"/>
+      <c r="S35" s="85"/>
+      <c r="T35" s="85"/>
+      <c r="U35" s="85"/>
+      <c r="V35" s="94"/>
       <c r="W35" s="1"/>
     </row>
     <row r="36" spans="1:23" ht="13.2">
       <c r="A36" s="1"/>
-      <c r="B36" s="89"/>
-      <c r="C36" s="81"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="81"/>
-      <c r="F36" s="81"/>
-      <c r="G36" s="81"/>
-      <c r="H36" s="81"/>
-      <c r="I36" s="81"/>
-      <c r="J36" s="81"/>
-      <c r="K36" s="81"/>
-      <c r="L36" s="81"/>
-      <c r="M36" s="81"/>
-      <c r="N36" s="81"/>
-      <c r="O36" s="81"/>
-      <c r="P36" s="81"/>
-      <c r="Q36" s="81"/>
-      <c r="R36" s="81"/>
-      <c r="S36" s="81"/>
-      <c r="T36" s="81"/>
-      <c r="U36" s="81"/>
-      <c r="V36" s="90"/>
+      <c r="B36" s="93"/>
+      <c r="C36" s="85"/>
+      <c r="D36" s="85"/>
+      <c r="E36" s="85"/>
+      <c r="F36" s="85"/>
+      <c r="G36" s="85"/>
+      <c r="H36" s="85"/>
+      <c r="I36" s="85"/>
+      <c r="J36" s="85"/>
+      <c r="K36" s="85"/>
+      <c r="L36" s="85"/>
+      <c r="M36" s="85"/>
+      <c r="N36" s="85"/>
+      <c r="O36" s="85"/>
+      <c r="P36" s="85"/>
+      <c r="Q36" s="85"/>
+      <c r="R36" s="85"/>
+      <c r="S36" s="85"/>
+      <c r="T36" s="85"/>
+      <c r="U36" s="85"/>
+      <c r="V36" s="94"/>
       <c r="W36" s="1"/>
     </row>
     <row r="37" spans="1:23" ht="13.2">
       <c r="A37" s="1"/>
-      <c r="B37" s="89"/>
-      <c r="C37" s="81"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="81"/>
-      <c r="G37" s="81"/>
-      <c r="H37" s="81"/>
-      <c r="I37" s="81"/>
-      <c r="J37" s="81"/>
-      <c r="K37" s="81"/>
-      <c r="L37" s="81"/>
-      <c r="M37" s="81"/>
-      <c r="N37" s="81"/>
-      <c r="O37" s="81"/>
-      <c r="P37" s="81"/>
-      <c r="Q37" s="81"/>
-      <c r="R37" s="81"/>
-      <c r="S37" s="81"/>
-      <c r="T37" s="81"/>
-      <c r="U37" s="81"/>
-      <c r="V37" s="90"/>
+      <c r="B37" s="93"/>
+      <c r="C37" s="85"/>
+      <c r="D37" s="85"/>
+      <c r="E37" s="85"/>
+      <c r="F37" s="85"/>
+      <c r="G37" s="85"/>
+      <c r="H37" s="85"/>
+      <c r="I37" s="85"/>
+      <c r="J37" s="85"/>
+      <c r="K37" s="85"/>
+      <c r="L37" s="85"/>
+      <c r="M37" s="85"/>
+      <c r="N37" s="85"/>
+      <c r="O37" s="85"/>
+      <c r="P37" s="85"/>
+      <c r="Q37" s="85"/>
+      <c r="R37" s="85"/>
+      <c r="S37" s="85"/>
+      <c r="T37" s="85"/>
+      <c r="U37" s="85"/>
+      <c r="V37" s="94"/>
       <c r="W37" s="1"/>
     </row>
     <row r="38" spans="1:23" ht="13.2">
       <c r="A38" s="1"/>
-      <c r="B38" s="89"/>
-      <c r="C38" s="81"/>
-      <c r="D38" s="81"/>
-      <c r="E38" s="81"/>
-      <c r="F38" s="81"/>
-      <c r="G38" s="81"/>
-      <c r="H38" s="81"/>
-      <c r="I38" s="81"/>
-      <c r="J38" s="81"/>
-      <c r="K38" s="81"/>
-      <c r="L38" s="81"/>
-      <c r="M38" s="81"/>
-      <c r="N38" s="81"/>
-      <c r="O38" s="81"/>
-      <c r="P38" s="81"/>
-      <c r="Q38" s="81"/>
-      <c r="R38" s="81"/>
-      <c r="S38" s="81"/>
-      <c r="T38" s="81"/>
-      <c r="U38" s="81"/>
-      <c r="V38" s="90"/>
+      <c r="B38" s="93"/>
+      <c r="C38" s="85"/>
+      <c r="D38" s="85"/>
+      <c r="E38" s="85"/>
+      <c r="F38" s="85"/>
+      <c r="G38" s="85"/>
+      <c r="H38" s="85"/>
+      <c r="I38" s="85"/>
+      <c r="J38" s="85"/>
+      <c r="K38" s="85"/>
+      <c r="L38" s="85"/>
+      <c r="M38" s="85"/>
+      <c r="N38" s="85"/>
+      <c r="O38" s="85"/>
+      <c r="P38" s="85"/>
+      <c r="Q38" s="85"/>
+      <c r="R38" s="85"/>
+      <c r="S38" s="85"/>
+      <c r="T38" s="85"/>
+      <c r="U38" s="85"/>
+      <c r="V38" s="94"/>
       <c r="W38" s="1"/>
     </row>
     <row r="39" spans="1:23" ht="13.2">
       <c r="A39" s="1"/>
-      <c r="B39" s="89"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
-      <c r="G39" s="81"/>
-      <c r="H39" s="81"/>
-      <c r="I39" s="81"/>
-      <c r="J39" s="81"/>
-      <c r="K39" s="81"/>
-      <c r="L39" s="81"/>
-      <c r="M39" s="81"/>
-      <c r="N39" s="81"/>
-      <c r="O39" s="81"/>
-      <c r="P39" s="81"/>
-      <c r="Q39" s="81"/>
-      <c r="R39" s="81"/>
-      <c r="S39" s="81"/>
-      <c r="T39" s="81"/>
-      <c r="U39" s="81"/>
-      <c r="V39" s="90"/>
+      <c r="B39" s="93"/>
+      <c r="C39" s="85"/>
+      <c r="D39" s="85"/>
+      <c r="E39" s="85"/>
+      <c r="F39" s="85"/>
+      <c r="G39" s="85"/>
+      <c r="H39" s="85"/>
+      <c r="I39" s="85"/>
+      <c r="J39" s="85"/>
+      <c r="K39" s="85"/>
+      <c r="L39" s="85"/>
+      <c r="M39" s="85"/>
+      <c r="N39" s="85"/>
+      <c r="O39" s="85"/>
+      <c r="P39" s="85"/>
+      <c r="Q39" s="85"/>
+      <c r="R39" s="85"/>
+      <c r="S39" s="85"/>
+      <c r="T39" s="85"/>
+      <c r="U39" s="85"/>
+      <c r="V39" s="94"/>
       <c r="W39" s="1"/>
     </row>
     <row r="40" spans="1:23" ht="13.2">
       <c r="A40" s="1"/>
-      <c r="B40" s="89"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="81"/>
-      <c r="G40" s="81"/>
-      <c r="H40" s="81"/>
-      <c r="I40" s="81"/>
-      <c r="J40" s="81"/>
-      <c r="K40" s="81"/>
-      <c r="L40" s="81"/>
-      <c r="M40" s="81"/>
-      <c r="N40" s="81"/>
-      <c r="O40" s="81"/>
-      <c r="P40" s="81"/>
-      <c r="Q40" s="81"/>
-      <c r="R40" s="81"/>
-      <c r="S40" s="81"/>
-      <c r="T40" s="81"/>
-      <c r="U40" s="81"/>
-      <c r="V40" s="90"/>
+      <c r="B40" s="93"/>
+      <c r="C40" s="85"/>
+      <c r="D40" s="85"/>
+      <c r="E40" s="85"/>
+      <c r="F40" s="85"/>
+      <c r="G40" s="85"/>
+      <c r="H40" s="85"/>
+      <c r="I40" s="85"/>
+      <c r="J40" s="85"/>
+      <c r="K40" s="85"/>
+      <c r="L40" s="85"/>
+      <c r="M40" s="85"/>
+      <c r="N40" s="85"/>
+      <c r="O40" s="85"/>
+      <c r="P40" s="85"/>
+      <c r="Q40" s="85"/>
+      <c r="R40" s="85"/>
+      <c r="S40" s="85"/>
+      <c r="T40" s="85"/>
+      <c r="U40" s="85"/>
+      <c r="V40" s="94"/>
       <c r="W40" s="1"/>
     </row>
     <row r="41" spans="1:23" ht="13.2">
       <c r="A41" s="1"/>
-      <c r="B41" s="89"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="81"/>
-      <c r="F41" s="81"/>
-      <c r="G41" s="81"/>
-      <c r="H41" s="81"/>
-      <c r="I41" s="81"/>
-      <c r="J41" s="81"/>
-      <c r="K41" s="81"/>
-      <c r="L41" s="81"/>
-      <c r="M41" s="81"/>
-      <c r="N41" s="81"/>
-      <c r="O41" s="81"/>
-      <c r="P41" s="81"/>
-      <c r="Q41" s="81"/>
-      <c r="R41" s="81"/>
-      <c r="S41" s="81"/>
-      <c r="T41" s="81"/>
-      <c r="U41" s="81"/>
-      <c r="V41" s="90"/>
+      <c r="B41" s="93"/>
+      <c r="C41" s="85"/>
+      <c r="D41" s="85"/>
+      <c r="E41" s="85"/>
+      <c r="F41" s="85"/>
+      <c r="G41" s="85"/>
+      <c r="H41" s="85"/>
+      <c r="I41" s="85"/>
+      <c r="J41" s="85"/>
+      <c r="K41" s="85"/>
+      <c r="L41" s="85"/>
+      <c r="M41" s="85"/>
+      <c r="N41" s="85"/>
+      <c r="O41" s="85"/>
+      <c r="P41" s="85"/>
+      <c r="Q41" s="85"/>
+      <c r="R41" s="85"/>
+      <c r="S41" s="85"/>
+      <c r="T41" s="85"/>
+      <c r="U41" s="85"/>
+      <c r="V41" s="94"/>
       <c r="W41" s="1"/>
     </row>
     <row r="42" spans="1:23" ht="13.2">
       <c r="A42" s="1"/>
-      <c r="B42" s="89"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="81"/>
-      <c r="E42" s="81"/>
-      <c r="F42" s="81"/>
-      <c r="G42" s="81"/>
-      <c r="H42" s="81"/>
-      <c r="I42" s="81"/>
-      <c r="J42" s="81"/>
-      <c r="K42" s="81"/>
-      <c r="L42" s="81"/>
-      <c r="M42" s="81"/>
-      <c r="N42" s="81"/>
-      <c r="O42" s="81"/>
-      <c r="P42" s="81"/>
-      <c r="Q42" s="81"/>
-      <c r="R42" s="81"/>
-      <c r="S42" s="81"/>
-      <c r="T42" s="81"/>
-      <c r="U42" s="81"/>
-      <c r="V42" s="90"/>
+      <c r="B42" s="93"/>
+      <c r="C42" s="85"/>
+      <c r="D42" s="85"/>
+      <c r="E42" s="85"/>
+      <c r="F42" s="85"/>
+      <c r="G42" s="85"/>
+      <c r="H42" s="85"/>
+      <c r="I42" s="85"/>
+      <c r="J42" s="85"/>
+      <c r="K42" s="85"/>
+      <c r="L42" s="85"/>
+      <c r="M42" s="85"/>
+      <c r="N42" s="85"/>
+      <c r="O42" s="85"/>
+      <c r="P42" s="85"/>
+      <c r="Q42" s="85"/>
+      <c r="R42" s="85"/>
+      <c r="S42" s="85"/>
+      <c r="T42" s="85"/>
+      <c r="U42" s="85"/>
+      <c r="V42" s="94"/>
       <c r="W42" s="1"/>
     </row>
     <row r="43" spans="1:23" ht="13.2">
       <c r="A43" s="1"/>
-      <c r="B43" s="89"/>
-      <c r="C43" s="81"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="81"/>
-      <c r="G43" s="81"/>
-      <c r="H43" s="81"/>
-      <c r="I43" s="81"/>
-      <c r="J43" s="81"/>
-      <c r="K43" s="81"/>
-      <c r="L43" s="81"/>
-      <c r="M43" s="81"/>
-      <c r="N43" s="81"/>
-      <c r="O43" s="81"/>
-      <c r="P43" s="81"/>
-      <c r="Q43" s="81"/>
-      <c r="R43" s="81"/>
-      <c r="S43" s="81"/>
-      <c r="T43" s="81"/>
-      <c r="U43" s="81"/>
-      <c r="V43" s="90"/>
+      <c r="B43" s="93"/>
+      <c r="C43" s="85"/>
+      <c r="D43" s="85"/>
+      <c r="E43" s="85"/>
+      <c r="F43" s="85"/>
+      <c r="G43" s="85"/>
+      <c r="H43" s="85"/>
+      <c r="I43" s="85"/>
+      <c r="J43" s="85"/>
+      <c r="K43" s="85"/>
+      <c r="L43" s="85"/>
+      <c r="M43" s="85"/>
+      <c r="N43" s="85"/>
+      <c r="O43" s="85"/>
+      <c r="P43" s="85"/>
+      <c r="Q43" s="85"/>
+      <c r="R43" s="85"/>
+      <c r="S43" s="85"/>
+      <c r="T43" s="85"/>
+      <c r="U43" s="85"/>
+      <c r="V43" s="94"/>
       <c r="W43" s="1"/>
     </row>
     <row r="44" spans="1:23" ht="13.2">
       <c r="A44" s="1"/>
-      <c r="B44" s="89"/>
-      <c r="C44" s="81"/>
-      <c r="D44" s="81"/>
-      <c r="E44" s="81"/>
-      <c r="F44" s="81"/>
-      <c r="G44" s="81"/>
-      <c r="H44" s="81"/>
-      <c r="I44" s="81"/>
-      <c r="J44" s="81"/>
-      <c r="K44" s="81"/>
-      <c r="L44" s="81"/>
-      <c r="M44" s="81"/>
-      <c r="N44" s="81"/>
-      <c r="O44" s="81"/>
-      <c r="P44" s="81"/>
-      <c r="Q44" s="81"/>
-      <c r="R44" s="81"/>
-      <c r="S44" s="81"/>
-      <c r="T44" s="81"/>
-      <c r="U44" s="81"/>
-      <c r="V44" s="90"/>
+      <c r="B44" s="93"/>
+      <c r="C44" s="85"/>
+      <c r="D44" s="85"/>
+      <c r="E44" s="85"/>
+      <c r="F44" s="85"/>
+      <c r="G44" s="85"/>
+      <c r="H44" s="85"/>
+      <c r="I44" s="85"/>
+      <c r="J44" s="85"/>
+      <c r="K44" s="85"/>
+      <c r="L44" s="85"/>
+      <c r="M44" s="85"/>
+      <c r="N44" s="85"/>
+      <c r="O44" s="85"/>
+      <c r="P44" s="85"/>
+      <c r="Q44" s="85"/>
+      <c r="R44" s="85"/>
+      <c r="S44" s="85"/>
+      <c r="T44" s="85"/>
+      <c r="U44" s="85"/>
+      <c r="V44" s="94"/>
       <c r="W44" s="1"/>
     </row>
     <row r="45" spans="1:23" ht="13.2">
       <c r="A45" s="1"/>
-      <c r="B45" s="89"/>
-      <c r="C45" s="81"/>
-      <c r="D45" s="81"/>
-      <c r="E45" s="81"/>
-      <c r="F45" s="81"/>
-      <c r="G45" s="81"/>
-      <c r="H45" s="81"/>
-      <c r="I45" s="81"/>
-      <c r="J45" s="81"/>
-      <c r="K45" s="81"/>
-      <c r="L45" s="81"/>
-      <c r="M45" s="81"/>
-      <c r="N45" s="81"/>
-      <c r="O45" s="81"/>
-      <c r="P45" s="81"/>
-      <c r="Q45" s="81"/>
-      <c r="R45" s="81"/>
-      <c r="S45" s="81"/>
-      <c r="T45" s="81"/>
-      <c r="U45" s="81"/>
-      <c r="V45" s="90"/>
+      <c r="B45" s="93"/>
+      <c r="C45" s="85"/>
+      <c r="D45" s="85"/>
+      <c r="E45" s="85"/>
+      <c r="F45" s="85"/>
+      <c r="G45" s="85"/>
+      <c r="H45" s="85"/>
+      <c r="I45" s="85"/>
+      <c r="J45" s="85"/>
+      <c r="K45" s="85"/>
+      <c r="L45" s="85"/>
+      <c r="M45" s="85"/>
+      <c r="N45" s="85"/>
+      <c r="O45" s="85"/>
+      <c r="P45" s="85"/>
+      <c r="Q45" s="85"/>
+      <c r="R45" s="85"/>
+      <c r="S45" s="85"/>
+      <c r="T45" s="85"/>
+      <c r="U45" s="85"/>
+      <c r="V45" s="94"/>
       <c r="W45" s="1"/>
     </row>
     <row r="46" spans="1:23" ht="13.2">
       <c r="A46" s="1"/>
-      <c r="B46" s="89"/>
-      <c r="C46" s="81"/>
-      <c r="D46" s="81"/>
-      <c r="E46" s="81"/>
-      <c r="F46" s="81"/>
-      <c r="G46" s="81"/>
-      <c r="H46" s="81"/>
-      <c r="I46" s="81"/>
-      <c r="J46" s="81"/>
-      <c r="K46" s="81"/>
-      <c r="L46" s="81"/>
-      <c r="M46" s="81"/>
-      <c r="N46" s="81"/>
-      <c r="O46" s="81"/>
-      <c r="P46" s="81"/>
-      <c r="Q46" s="81"/>
-      <c r="R46" s="81"/>
-      <c r="S46" s="81"/>
-      <c r="T46" s="81"/>
-      <c r="U46" s="81"/>
-      <c r="V46" s="90"/>
+      <c r="B46" s="93"/>
+      <c r="C46" s="85"/>
+      <c r="D46" s="85"/>
+      <c r="E46" s="85"/>
+      <c r="F46" s="85"/>
+      <c r="G46" s="85"/>
+      <c r="H46" s="85"/>
+      <c r="I46" s="85"/>
+      <c r="J46" s="85"/>
+      <c r="K46" s="85"/>
+      <c r="L46" s="85"/>
+      <c r="M46" s="85"/>
+      <c r="N46" s="85"/>
+      <c r="O46" s="85"/>
+      <c r="P46" s="85"/>
+      <c r="Q46" s="85"/>
+      <c r="R46" s="85"/>
+      <c r="S46" s="85"/>
+      <c r="T46" s="85"/>
+      <c r="U46" s="85"/>
+      <c r="V46" s="94"/>
       <c r="W46" s="1"/>
     </row>
     <row r="47" spans="1:23" ht="13.2">
       <c r="A47" s="1"/>
-      <c r="B47" s="91"/>
-      <c r="C47" s="92"/>
-      <c r="D47" s="92"/>
-      <c r="E47" s="92"/>
-      <c r="F47" s="92"/>
-      <c r="G47" s="92"/>
-      <c r="H47" s="92"/>
-      <c r="I47" s="92"/>
-      <c r="J47" s="92"/>
-      <c r="K47" s="92"/>
-      <c r="L47" s="92"/>
-      <c r="M47" s="92"/>
-      <c r="N47" s="92"/>
-      <c r="O47" s="92"/>
-      <c r="P47" s="92"/>
-      <c r="Q47" s="92"/>
-      <c r="R47" s="92"/>
-      <c r="S47" s="92"/>
-      <c r="T47" s="92"/>
-      <c r="U47" s="92"/>
-      <c r="V47" s="93"/>
+      <c r="B47" s="95"/>
+      <c r="C47" s="96"/>
+      <c r="D47" s="96"/>
+      <c r="E47" s="96"/>
+      <c r="F47" s="96"/>
+      <c r="G47" s="96"/>
+      <c r="H47" s="96"/>
+      <c r="I47" s="96"/>
+      <c r="J47" s="96"/>
+      <c r="K47" s="96"/>
+      <c r="L47" s="96"/>
+      <c r="M47" s="96"/>
+      <c r="N47" s="96"/>
+      <c r="O47" s="96"/>
+      <c r="P47" s="96"/>
+      <c r="Q47" s="96"/>
+      <c r="R47" s="96"/>
+      <c r="S47" s="96"/>
+      <c r="T47" s="96"/>
+      <c r="U47" s="96"/>
+      <c r="V47" s="97"/>
       <c r="W47" s="1"/>
     </row>
     <row r="48" spans="1:23" ht="13.2">
@@ -3706,10 +3863,10 @@
   <dimension ref="A1:AN994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D48" sqref="D48"/>
+      <selection pane="bottomRight" activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -46757,13 +46914,7 @@
       <c r="AN994" s="49"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="E3:E994" xr:uid="{00000000-0002-0000-0300-000000000000}">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="AC2:AJ994 E2 D2:D994" xr:uid="{00000000-0002-0000-0300-000001000000}">
-      <formula1>#REF!</formula1>
-    </dataValidation>
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{EF251A3B-552F-438A-8A9A-6C4288DF2CE6}">
       <formula1>"Arcane, Earth, Fire, Ice, Light, Lightning, Nature, Plague, Shadow, Wind, Water"</formula1>
     </dataValidation>
@@ -46775,10 +46926,566 @@
     <hyperlink ref="U52" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
+          <x14:formula1>
+            <xm:f>validation!$B$2:$B$100</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D994</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Unrecognised pronoun" error="pronoun not in list" xr:uid="{6BDABD9C-CDB7-4C51-BB12-4CAD33033EB7}">
+          <x14:formula1>
+            <xm:f>validation!$E$2:$E$100</xm:f>
+          </x14:formula1>
+          <xm:sqref>AG2:AJ1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" errorTitle="Unknown flag" error="flag is not on list" xr:uid="{B5CD4B24-DAC3-4789-9289-48E9AAF45EFF}">
+          <x14:formula1>
+            <xm:f>validation!$D$2:$D$1000</xm:f>
+          </x14:formula1>
+          <xm:sqref>AC2:AF1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9BBA1311-87F7-4FD1-A6D2-2668448E4F45}">
+          <x14:formula1>
+            <xm:f>validation!$C$2:$C$100</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C02D28-655F-4926-87D2-41F48C8F42BF}">
+  <dimension ref="A1:E73"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="55" t="s">
+        <v>271</v>
+      </c>
+      <c r="B1" s="55" t="s">
+        <v>272</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1" s="82" t="s">
+        <v>300</v>
+      </c>
+      <c r="E1" s="82" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="80" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="81" t="s">
+        <v>309</v>
+      </c>
+      <c r="E2" s="81" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C3" s="80" t="s">
+        <v>341</v>
+      </c>
+      <c r="D3" s="81" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="81" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C4" s="80" t="s">
+        <v>342</v>
+      </c>
+      <c r="D4" s="81" t="s">
+        <v>331</v>
+      </c>
+      <c r="E4" s="81" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C5" s="80" t="s">
+        <v>343</v>
+      </c>
+      <c r="D5" s="81" t="s">
+        <v>230</v>
+      </c>
+      <c r="E5" s="81" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
+        <v>305</v>
+      </c>
+      <c r="C6" s="80" t="s">
+        <v>344</v>
+      </c>
+      <c r="D6" s="81" t="s">
+        <v>310</v>
+      </c>
+      <c r="E6" s="81" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
+        <v>306</v>
+      </c>
+      <c r="C7" s="80" t="s">
+        <v>345</v>
+      </c>
+      <c r="D7" s="81" t="s">
+        <v>311</v>
+      </c>
+      <c r="E7" s="81" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B8" t="s">
+        <v>307</v>
+      </c>
+      <c r="D8" s="81" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="81" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" t="s">
+        <v>308</v>
+      </c>
+      <c r="D9" s="81" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" s="81" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="81" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="81" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="81" t="s">
+        <v>237</v>
+      </c>
+      <c r="E11" s="81"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="83" t="s">
+        <v>332</v>
+      </c>
+      <c r="E12" s="81"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="80" t="s">
+        <v>339</v>
+      </c>
+      <c r="D13" s="81" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="81"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="80" t="s">
+        <v>340</v>
+      </c>
+      <c r="D14" s="81" t="s">
+        <v>312</v>
+      </c>
+      <c r="E14" s="81"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="D15" s="81" t="s">
+        <v>313</v>
+      </c>
+      <c r="E15" s="81"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="D16" s="81" t="s">
+        <v>188</v>
+      </c>
+      <c r="E16" s="81"/>
+    </row>
+    <row r="17" spans="4:5">
+      <c r="D17" s="81" t="s">
+        <v>314</v>
+      </c>
+      <c r="E17" s="81"/>
+    </row>
+    <row r="18" spans="4:5">
+      <c r="D18" s="81" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="81"/>
+    </row>
+    <row r="19" spans="4:5">
+      <c r="D19" s="81" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="81"/>
+    </row>
+    <row r="20" spans="4:5">
+      <c r="D20" s="81" t="s">
+        <v>315</v>
+      </c>
+      <c r="E20" s="81"/>
+    </row>
+    <row r="21" spans="4:5">
+      <c r="D21" s="81" t="s">
+        <v>133</v>
+      </c>
+      <c r="E21" s="81"/>
+    </row>
+    <row r="22" spans="4:5">
+      <c r="D22" s="81" t="s">
+        <v>207</v>
+      </c>
+      <c r="E22" s="81"/>
+    </row>
+    <row r="23" spans="4:5">
+      <c r="D23" s="81" t="s">
+        <v>316</v>
+      </c>
+      <c r="E23" s="81"/>
+    </row>
+    <row r="24" spans="4:5">
+      <c r="D24" s="81" t="s">
+        <v>317</v>
+      </c>
+      <c r="E24" s="81"/>
+    </row>
+    <row r="25" spans="4:5">
+      <c r="D25" s="81" t="s">
+        <v>318</v>
+      </c>
+      <c r="E25" s="81"/>
+    </row>
+    <row r="26" spans="4:5">
+      <c r="D26" s="81" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="81"/>
+    </row>
+    <row r="27" spans="4:5">
+      <c r="D27" s="81" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" s="81"/>
+    </row>
+    <row r="28" spans="4:5">
+      <c r="D28" s="81" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="81"/>
+    </row>
+    <row r="29" spans="4:5">
+      <c r="D29" s="81" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="81"/>
+    </row>
+    <row r="30" spans="4:5">
+      <c r="D30" s="81" t="s">
+        <v>319</v>
+      </c>
+      <c r="E30" s="81"/>
+    </row>
+    <row r="31" spans="4:5">
+      <c r="D31" s="81" t="s">
+        <v>330</v>
+      </c>
+      <c r="E31" s="81"/>
+    </row>
+    <row r="32" spans="4:5">
+      <c r="D32" s="81" t="s">
+        <v>320</v>
+      </c>
+      <c r="E32" s="81"/>
+    </row>
+    <row r="33" spans="4:5">
+      <c r="D33" s="81" t="s">
+        <v>321</v>
+      </c>
+      <c r="E33" s="81"/>
+    </row>
+    <row r="34" spans="4:5">
+      <c r="D34" s="81" t="s">
+        <v>145</v>
+      </c>
+      <c r="E34" s="81"/>
+    </row>
+    <row r="35" spans="4:5">
+      <c r="D35" s="81" t="s">
+        <v>323</v>
+      </c>
+      <c r="E35" s="81"/>
+    </row>
+    <row r="36" spans="4:5">
+      <c r="D36" s="81" t="s">
+        <v>322</v>
+      </c>
+      <c r="E36" s="81"/>
+    </row>
+    <row r="37" spans="4:5">
+      <c r="D37" s="81" t="s">
+        <v>329</v>
+      </c>
+      <c r="E37" s="81"/>
+    </row>
+    <row r="38" spans="4:5">
+      <c r="D38" s="81" t="s">
+        <v>324</v>
+      </c>
+      <c r="E38" s="81"/>
+    </row>
+    <row r="39" spans="4:5">
+      <c r="D39" s="81" t="s">
+        <v>325</v>
+      </c>
+      <c r="E39" s="81"/>
+    </row>
+    <row r="40" spans="4:5">
+      <c r="D40" s="81" t="s">
+        <v>213</v>
+      </c>
+      <c r="E40" s="81"/>
+    </row>
+    <row r="41" spans="4:5">
+      <c r="D41" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" s="81"/>
+    </row>
+    <row r="42" spans="4:5">
+      <c r="D42" s="81" t="s">
+        <v>326</v>
+      </c>
+      <c r="E42" s="81"/>
+    </row>
+    <row r="43" spans="4:5">
+      <c r="D43" s="83" t="s">
+        <v>333</v>
+      </c>
+      <c r="E43" s="81"/>
+    </row>
+    <row r="44" spans="4:5">
+      <c r="D44" s="83" t="s">
+        <v>334</v>
+      </c>
+      <c r="E44" s="81"/>
+    </row>
+    <row r="45" spans="4:5">
+      <c r="D45" s="81" t="s">
+        <v>58</v>
+      </c>
+      <c r="E45" s="81"/>
+    </row>
+    <row r="46" spans="4:5">
+      <c r="D46" s="83" t="s">
+        <v>299</v>
+      </c>
+      <c r="E46" s="81"/>
+    </row>
+    <row r="47" spans="4:5">
+      <c r="D47" s="81" t="s">
+        <v>327</v>
+      </c>
+      <c r="E47" s="81"/>
+    </row>
+    <row r="48" spans="4:5">
+      <c r="D48" s="81" t="s">
+        <v>83</v>
+      </c>
+      <c r="E48" s="81"/>
+    </row>
+    <row r="49" spans="4:5">
+      <c r="D49" s="81" t="s">
+        <v>138</v>
+      </c>
+      <c r="E49" s="81"/>
+    </row>
+    <row r="50" spans="4:5">
+      <c r="D50" s="81" t="s">
+        <v>328</v>
+      </c>
+      <c r="E50" s="81"/>
+    </row>
+    <row r="51" spans="4:5">
+      <c r="D51" s="81"/>
+      <c r="E51" s="81"/>
+    </row>
+    <row r="52" spans="4:5">
+      <c r="D52" s="81"/>
+      <c r="E52" s="81"/>
+    </row>
+    <row r="53" spans="4:5">
+      <c r="D53" s="81"/>
+      <c r="E53" s="81"/>
+    </row>
+    <row r="54" spans="4:5">
+      <c r="D54" s="81"/>
+      <c r="E54" s="81"/>
+    </row>
+    <row r="55" spans="4:5">
+      <c r="D55" s="81"/>
+      <c r="E55" s="81"/>
+    </row>
+    <row r="56" spans="4:5">
+      <c r="D56" s="81"/>
+      <c r="E56" s="81"/>
+    </row>
+    <row r="57" spans="4:5">
+      <c r="D57" s="81"/>
+      <c r="E57" s="81"/>
+    </row>
+    <row r="58" spans="4:5">
+      <c r="D58" s="81"/>
+      <c r="E58" s="81"/>
+    </row>
+    <row r="59" spans="4:5">
+      <c r="D59" s="81"/>
+      <c r="E59" s="81"/>
+    </row>
+    <row r="60" spans="4:5">
+      <c r="D60" s="81"/>
+      <c r="E60" s="81"/>
+    </row>
+    <row r="61" spans="4:5">
+      <c r="D61" s="81"/>
+      <c r="E61" s="81"/>
+    </row>
+    <row r="62" spans="4:5">
+      <c r="D62" s="81"/>
+      <c r="E62" s="81"/>
+    </row>
+    <row r="63" spans="4:5">
+      <c r="D63" s="81"/>
+      <c r="E63" s="81"/>
+    </row>
+    <row r="64" spans="4:5">
+      <c r="D64" s="81"/>
+      <c r="E64" s="81"/>
+    </row>
+    <row r="65" spans="4:5">
+      <c r="D65" s="81"/>
+      <c r="E65" s="81"/>
+    </row>
+    <row r="66" spans="4:5">
+      <c r="D66" s="81"/>
+      <c r="E66" s="81"/>
+    </row>
+    <row r="67" spans="4:5">
+      <c r="D67" s="81"/>
+      <c r="E67" s="81"/>
+    </row>
+    <row r="68" spans="4:5">
+      <c r="D68" s="81"/>
+      <c r="E68" s="81"/>
+    </row>
+    <row r="69" spans="4:5">
+      <c r="D69" s="81"/>
+      <c r="E69" s="81"/>
+    </row>
+    <row r="70" spans="4:5">
+      <c r="D70" s="81"/>
+      <c r="E70" s="81"/>
+    </row>
+    <row r="71" spans="4:5">
+      <c r="D71" s="81"/>
+      <c r="E71" s="81"/>
+    </row>
+    <row r="72" spans="4:5">
+      <c r="D72" s="81"/>
+      <c r="E72" s="81"/>
+    </row>
+    <row r="73" spans="4:5">
+      <c r="D73" s="81"/>
+      <c r="E73" s="81"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:E11">
+    <sortCondition ref="E2:E11"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
bios up to Fen
</commit_message>
<xml_diff>
--- a/bio_info.xlsx
+++ b/bio_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isobe\fr\dragon-bios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFF545D-1B18-4B4E-AAEB-C15326FB812B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74174CBF-0E93-4B7C-93FF-3FFC634BF968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -283,7 +283,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="302">
   <si>
     <t>Dragon Info</t>
   </si>
@@ -1207,6 +1207,9 @@
   </si>
   <si>
     <t>Scrolls L</t>
+  </si>
+  <si>
+    <t>Unearned Achievements</t>
   </si>
 </sst>
 </file>
@@ -3728,10 +3731,10 @@
   <dimension ref="A1:AJ994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
+      <selection pane="bottomRight" activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.95" customHeight="1"/>
@@ -4181,7 +4184,9 @@
       <c r="R6" s="93"/>
       <c r="S6" s="92"/>
       <c r="T6" s="92"/>
-      <c r="U6" s="93"/>
+      <c r="U6" s="93" t="s">
+        <v>301</v>
+      </c>
       <c r="V6" s="93"/>
       <c r="W6" s="92"/>
       <c r="X6" s="93"/>

</xml_diff>

<commit_message>
add extra spacing when section title is followed by [center]
</commit_message>
<xml_diff>
--- a/bio_info.xlsx
+++ b/bio_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isobe\fr\dragon-bios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C71C2B-ACF6-464D-91BD-4DD1AC154690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E267455C-FDF1-4F9E-886B-6A83FBD59292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -708,9 +708,6 @@
     <t>Insert missing apostrophe to aquagraph alt text</t>
   </si>
   <si>
-    <t>Ice Pixel Kitties[br][br]</t>
-  </si>
-  <si>
     <t>Liquorice</t>
   </si>
   <si>
@@ -1228,6 +1225,9 @@
   </si>
   <si>
     <t>Tiger Treats</t>
+  </si>
+  <si>
+    <t>Ice Pixel Kitties</t>
   </si>
 </sst>
 </file>
@@ -3755,10 +3755,10 @@
   <dimension ref="A1:AK994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomRight" activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.95" customHeight="1"/>
@@ -3790,121 +3790,121 @@
   <sheetData>
     <row r="1" spans="1:37" s="105" customFormat="1" ht="13.95" customHeight="1">
       <c r="A1" s="56" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>301</v>
+      </c>
+      <c r="C1" s="57" t="s">
         <v>228</v>
       </c>
-      <c r="B1" s="60" t="s">
-        <v>302</v>
-      </c>
-      <c r="C1" s="57" t="s">
+      <c r="D1" s="58" t="s">
         <v>229</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="E1" s="58" t="s">
         <v>230</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="F1" s="58" t="s">
         <v>231</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="G1" s="58" t="s">
         <v>232</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="H1" s="59" t="s">
+        <v>219</v>
+      </c>
+      <c r="I1" s="60" t="s">
+        <v>218</v>
+      </c>
+      <c r="J1" s="61" t="s">
+        <v>220</v>
+      </c>
+      <c r="K1" s="59" t="s">
+        <v>221</v>
+      </c>
+      <c r="L1" s="60" t="s">
+        <v>222</v>
+      </c>
+      <c r="M1" s="61" t="s">
+        <v>223</v>
+      </c>
+      <c r="N1" s="59" t="s">
+        <v>224</v>
+      </c>
+      <c r="O1" s="60" t="s">
+        <v>225</v>
+      </c>
+      <c r="P1" s="61" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q1" s="62" t="s">
         <v>233</v>
       </c>
-      <c r="H1" s="59" t="s">
-        <v>220</v>
-      </c>
-      <c r="I1" s="60" t="s">
-        <v>219</v>
-      </c>
-      <c r="J1" s="61" t="s">
-        <v>221</v>
-      </c>
-      <c r="K1" s="59" t="s">
-        <v>222</v>
-      </c>
-      <c r="L1" s="60" t="s">
-        <v>223</v>
-      </c>
-      <c r="M1" s="61" t="s">
-        <v>224</v>
-      </c>
-      <c r="N1" s="59" t="s">
-        <v>225</v>
-      </c>
-      <c r="O1" s="60" t="s">
-        <v>226</v>
-      </c>
-      <c r="P1" s="61" t="s">
-        <v>227</v>
-      </c>
-      <c r="Q1" s="62" t="s">
+      <c r="R1" s="63" t="s">
         <v>234</v>
       </c>
-      <c r="R1" s="63" t="s">
+      <c r="S1" s="62" t="s">
         <v>235</v>
       </c>
-      <c r="S1" s="62" t="s">
+      <c r="T1" s="58" t="s">
         <v>236</v>
       </c>
-      <c r="T1" s="58" t="s">
+      <c r="U1" s="58" t="s">
         <v>237</v>
       </c>
-      <c r="U1" s="58" t="s">
+      <c r="V1" s="62" t="s">
+        <v>248</v>
+      </c>
+      <c r="W1" s="62" t="s">
+        <v>249</v>
+      </c>
+      <c r="X1" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="Y1" s="62" t="s">
+        <v>251</v>
+      </c>
+      <c r="Z1" s="62" t="s">
         <v>238</v>
       </c>
-      <c r="V1" s="62" t="s">
-        <v>249</v>
-      </c>
-      <c r="W1" s="62" t="s">
-        <v>250</v>
-      </c>
-      <c r="X1" s="58" t="s">
-        <v>251</v>
-      </c>
-      <c r="Y1" s="62" t="s">
+      <c r="AA1" s="58" t="s">
+        <v>239</v>
+      </c>
+      <c r="AB1" s="58" t="s">
+        <v>240</v>
+      </c>
+      <c r="AC1" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="AD1" s="62" t="s">
+        <v>242</v>
+      </c>
+      <c r="AE1" s="58" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF1" s="58" t="s">
+        <v>244</v>
+      </c>
+      <c r="AG1" s="58" t="s">
+        <v>245</v>
+      </c>
+      <c r="AH1" s="57" t="s">
+        <v>246</v>
+      </c>
+      <c r="AI1" s="64" t="s">
+        <v>247</v>
+      </c>
+      <c r="AJ1" s="57" t="s">
         <v>252</v>
-      </c>
-      <c r="Z1" s="62" t="s">
-        <v>239</v>
-      </c>
-      <c r="AA1" s="58" t="s">
-        <v>240</v>
-      </c>
-      <c r="AB1" s="58" t="s">
-        <v>241</v>
-      </c>
-      <c r="AC1" s="58" t="s">
-        <v>242</v>
-      </c>
-      <c r="AD1" s="62" t="s">
-        <v>243</v>
-      </c>
-      <c r="AE1" s="58" t="s">
-        <v>244</v>
-      </c>
-      <c r="AF1" s="58" t="s">
-        <v>245</v>
-      </c>
-      <c r="AG1" s="58" t="s">
-        <v>246</v>
-      </c>
-      <c r="AH1" s="57" t="s">
-        <v>247</v>
-      </c>
-      <c r="AI1" s="64" t="s">
-        <v>248</v>
-      </c>
-      <c r="AJ1" s="57" t="s">
-        <v>253</v>
       </c>
       <c r="AK1" s="65"/>
     </row>
     <row r="2" spans="1:37" ht="13.95" customHeight="1">
       <c r="A2" s="67" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B2" s="81" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C2" s="68"/>
       <c r="D2" s="69" t="s">
@@ -3954,10 +3954,10 @@
     </row>
     <row r="3" spans="1:37" ht="13.95" customHeight="1">
       <c r="A3" s="67" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C3" s="68"/>
       <c r="D3" s="69" t="s">
@@ -3988,7 +3988,7 @@
       <c r="U3" s="69"/>
       <c r="V3" s="70"/>
       <c r="W3" s="70" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="X3" s="69"/>
       <c r="Y3" s="70"/>
@@ -4010,7 +4010,7 @@
         <v>130</v>
       </c>
       <c r="B4" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C4" s="68" t="s">
         <v>131</v>
@@ -4062,14 +4062,14 @@
     </row>
     <row r="5" spans="1:37" ht="13.95" customHeight="1">
       <c r="A5" s="67" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B5" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C5" s="68"/>
       <c r="D5" s="69" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
@@ -4094,7 +4094,7 @@
       <c r="Y5" s="70"/>
       <c r="Z5" s="70"/>
       <c r="AA5" s="69" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AB5" s="69" t="s">
         <v>113</v>
@@ -4113,10 +4113,10 @@
     </row>
     <row r="6" spans="1:37" ht="13.95" customHeight="1">
       <c r="A6" s="67" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B6" s="81" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C6" s="68"/>
       <c r="D6" s="69" t="s">
@@ -4169,7 +4169,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="81" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C7" s="68"/>
       <c r="D7" s="69" t="s">
@@ -4205,7 +4205,7 @@
       <c r="T7" s="69"/>
       <c r="U7" s="69"/>
       <c r="V7" s="70" t="s">
-        <v>141</v>
+        <v>307</v>
       </c>
       <c r="W7" s="70"/>
       <c r="X7" s="69"/>
@@ -4230,7 +4230,7 @@
         <v>99</v>
       </c>
       <c r="B8" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C8" s="68" t="s">
         <v>102</v>
@@ -4295,7 +4295,7 @@
         <v>138</v>
       </c>
       <c r="B9" s="81" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C9" s="68"/>
       <c r="D9" s="69" t="s">
@@ -4356,7 +4356,7 @@
         <v>52</v>
       </c>
       <c r="B10" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C10" s="68" t="s">
         <v>63</v>
@@ -4425,7 +4425,7 @@
         <v>67</v>
       </c>
       <c r="B11" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C11" s="68" t="s">
         <v>68</v>
@@ -4485,10 +4485,10 @@
     </row>
     <row r="12" spans="1:37" ht="13.95" customHeight="1">
       <c r="A12" s="67" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B12" s="81" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C12" s="68"/>
       <c r="D12" s="69" t="s">
@@ -4540,10 +4540,10 @@
     </row>
     <row r="13" spans="1:37" ht="13.95" customHeight="1">
       <c r="A13" s="67" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B13" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C13" s="68"/>
       <c r="D13" s="69" t="s">
@@ -4591,16 +4591,16 @@
     </row>
     <row r="14" spans="1:37" ht="13.95" customHeight="1">
       <c r="A14" s="67" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" s="81" t="s">
+        <v>302</v>
+      </c>
+      <c r="C14" s="68" t="s">
         <v>192</v>
       </c>
-      <c r="B14" s="81" t="s">
-        <v>303</v>
-      </c>
-      <c r="C14" s="68" t="s">
-        <v>193</v>
-      </c>
       <c r="D14" s="69" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E14" s="69" t="s">
         <v>49</v>
@@ -4635,13 +4635,13 @@
         <v>113</v>
       </c>
       <c r="AC14" s="69" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AD14" s="70" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AE14" s="69" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AF14" s="69"/>
       <c r="AG14" s="69"/>
@@ -4652,13 +4652,13 @@
     </row>
     <row r="15" spans="1:37" ht="13.95" customHeight="1">
       <c r="A15" s="67" t="s">
+        <v>197</v>
+      </c>
+      <c r="B15" s="81" t="s">
+        <v>302</v>
+      </c>
+      <c r="C15" s="68" t="s">
         <v>198</v>
-      </c>
-      <c r="B15" s="81" t="s">
-        <v>303</v>
-      </c>
-      <c r="C15" s="68" t="s">
-        <v>199</v>
       </c>
       <c r="D15" s="69" t="s">
         <v>139</v>
@@ -4684,7 +4684,7 @@
       <c r="Q15" s="70"/>
       <c r="R15" s="69"/>
       <c r="S15" s="70" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="T15" s="69"/>
       <c r="U15" s="69"/>
@@ -4694,7 +4694,7 @@
       <c r="Y15" s="70"/>
       <c r="Z15" s="70"/>
       <c r="AA15" s="69" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB15" s="69" t="s">
         <v>57</v>
@@ -4718,7 +4718,7 @@
         <v>133</v>
       </c>
       <c r="B16" s="81" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C16" s="68" t="s">
         <v>134</v>
@@ -4781,7 +4781,7 @@
         <v>119</v>
       </c>
       <c r="B17" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C17" s="68" t="s">
         <v>120</v>
@@ -4839,14 +4839,14 @@
     </row>
     <row r="18" spans="1:37" ht="13.95" customHeight="1">
       <c r="A18" s="67" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B18" s="81" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C18" s="68"/>
       <c r="D18" s="69" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E18" s="69" t="s">
         <v>49</v>
@@ -4872,7 +4872,7 @@
       <c r="T18" s="69"/>
       <c r="U18" s="69"/>
       <c r="V18" s="70" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="W18" s="70"/>
       <c r="X18" s="69"/>
@@ -4892,13 +4892,13 @@
     </row>
     <row r="19" spans="1:37" ht="13.95" customHeight="1">
       <c r="A19" s="67" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B19" s="81" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C19" s="68" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D19" s="69" t="s">
         <v>7</v>
@@ -4913,7 +4913,7 @@
         <v>11</v>
       </c>
       <c r="H19" s="70" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I19" s="69" t="s">
         <v>76</v>
@@ -4933,7 +4933,7 @@
       <c r="T19" s="69"/>
       <c r="U19" s="69"/>
       <c r="V19" s="70" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="W19" s="70"/>
       <c r="X19" s="69"/>
@@ -4957,12 +4957,12 @@
     </row>
     <row r="20" spans="1:37" ht="13.95" customHeight="1">
       <c r="A20" s="67" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B20" s="81"/>
       <c r="C20" s="68"/>
       <c r="D20" s="69" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E20" s="69" t="s">
         <v>49</v>
@@ -4985,7 +4985,7 @@
       <c r="Q20" s="70"/>
       <c r="R20" s="69"/>
       <c r="S20" s="70" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T20" s="69"/>
       <c r="U20" s="69"/>
@@ -5004,16 +5004,16 @@
       <c r="AH20" s="70"/>
       <c r="AI20" s="72"/>
       <c r="AJ20" s="73" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AK20" s="65"/>
     </row>
     <row r="21" spans="1:37" ht="13.95" customHeight="1">
       <c r="A21" s="67" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B21" s="81" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C21" s="68"/>
       <c r="D21" s="69" t="s">
@@ -5057,7 +5057,7 @@
         <v>115</v>
       </c>
       <c r="AF21" s="69" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AG21" s="69"/>
       <c r="AH21" s="70"/>
@@ -5070,7 +5070,7 @@
         <v>124</v>
       </c>
       <c r="B22" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C22" s="68" t="s">
         <v>5</v>
@@ -5136,10 +5136,10 @@
     </row>
     <row r="23" spans="1:37" ht="13.95" customHeight="1">
       <c r="A23" s="67" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B23" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C23" s="68"/>
       <c r="D23" s="69" t="s">
@@ -5196,7 +5196,7 @@
         <v>92</v>
       </c>
       <c r="B24" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C24" s="68" t="s">
         <v>93</v>
@@ -5254,13 +5254,13 @@
     </row>
     <row r="25" spans="1:37" ht="13.95" customHeight="1">
       <c r="A25" s="67" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B25" s="81" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C25" s="68" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D25" s="69" t="s">
         <v>83</v>
@@ -5275,28 +5275,28 @@
         <v>11</v>
       </c>
       <c r="H25" s="70" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I25" s="69" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J25" s="71">
         <v>29446975</v>
       </c>
       <c r="K25" s="70" t="s">
+        <v>170</v>
+      </c>
+      <c r="L25" s="69" t="s">
         <v>171</v>
-      </c>
-      <c r="L25" s="69" t="s">
-        <v>172</v>
       </c>
       <c r="M25" s="71">
         <v>31679582</v>
       </c>
       <c r="N25" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="O25" s="69" t="s">
         <v>173</v>
-      </c>
-      <c r="O25" s="69" t="s">
-        <v>174</v>
       </c>
       <c r="P25" s="71">
         <v>33867433</v>
@@ -5313,7 +5313,7 @@
       <c r="Z25" s="70"/>
       <c r="AA25" s="69"/>
       <c r="AB25" s="69" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AC25" s="69"/>
       <c r="AD25" s="70" t="s">
@@ -5329,13 +5329,13 @@
     </row>
     <row r="26" spans="1:37" ht="13.95" customHeight="1">
       <c r="A26" s="67" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B26" s="81" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C26" s="68" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D26" s="69" t="s">
         <v>106</v>
@@ -5350,28 +5350,28 @@
         <v>11</v>
       </c>
       <c r="H26" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="I26" s="69" t="s">
         <v>175</v>
-      </c>
-      <c r="I26" s="69" t="s">
-        <v>176</v>
       </c>
       <c r="J26" s="71">
         <v>36097859</v>
       </c>
       <c r="K26" s="70" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L26" s="69" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M26" s="71">
         <v>29446975</v>
       </c>
       <c r="N26" s="70" t="s">
+        <v>170</v>
+      </c>
+      <c r="O26" s="69" t="s">
         <v>171</v>
-      </c>
-      <c r="O26" s="69" t="s">
-        <v>172</v>
       </c>
       <c r="P26" s="71">
         <v>31679582</v>
@@ -5388,7 +5388,7 @@
       <c r="Z26" s="70"/>
       <c r="AA26" s="69"/>
       <c r="AB26" s="69" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AC26" s="69"/>
       <c r="AD26" s="70" t="s">
@@ -5404,13 +5404,13 @@
     </row>
     <row r="27" spans="1:37" ht="13.95" customHeight="1">
       <c r="A27" s="67" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B27" s="81" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C27" s="68" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D27" s="69" t="s">
         <v>139</v>
@@ -5425,28 +5425,28 @@
         <v>11</v>
       </c>
       <c r="H27" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="I27" s="69" t="s">
         <v>173</v>
-      </c>
-      <c r="I27" s="69" t="s">
-        <v>174</v>
       </c>
       <c r="J27" s="71">
         <v>33867433</v>
       </c>
       <c r="K27" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="L27" s="69" t="s">
         <v>175</v>
-      </c>
-      <c r="L27" s="69" t="s">
-        <v>176</v>
       </c>
       <c r="M27" s="71">
         <v>36097859</v>
       </c>
       <c r="N27" s="70" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O27" s="69" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P27" s="71">
         <v>29446975</v>
@@ -5463,7 +5463,7 @@
       <c r="Z27" s="70"/>
       <c r="AA27" s="69"/>
       <c r="AB27" s="69" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AC27" s="69"/>
       <c r="AD27" s="70" t="s">
@@ -5481,16 +5481,16 @@
     </row>
     <row r="28" spans="1:37" ht="13.95" customHeight="1">
       <c r="A28" s="67" t="s">
+        <v>167</v>
+      </c>
+      <c r="B28" s="81" t="s">
+        <v>303</v>
+      </c>
+      <c r="C28" s="68" t="s">
         <v>168</v>
       </c>
-      <c r="B28" s="81" t="s">
-        <v>304</v>
-      </c>
-      <c r="C28" s="68" t="s">
+      <c r="D28" s="69" t="s">
         <v>169</v>
-      </c>
-      <c r="D28" s="69" t="s">
-        <v>170</v>
       </c>
       <c r="E28" s="69" t="s">
         <v>49</v>
@@ -5502,28 +5502,28 @@
         <v>11</v>
       </c>
       <c r="H28" s="70" t="s">
+        <v>170</v>
+      </c>
+      <c r="I28" s="69" t="s">
         <v>171</v>
-      </c>
-      <c r="I28" s="69" t="s">
-        <v>172</v>
       </c>
       <c r="J28" s="71">
         <v>31679582</v>
       </c>
       <c r="K28" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="L28" s="69" t="s">
         <v>173</v>
-      </c>
-      <c r="L28" s="69" t="s">
-        <v>174</v>
       </c>
       <c r="M28" s="71">
         <v>33867433</v>
       </c>
       <c r="N28" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="O28" s="69" t="s">
         <v>175</v>
-      </c>
-      <c r="O28" s="69" t="s">
-        <v>176</v>
       </c>
       <c r="P28" s="71">
         <v>36097859</v>
@@ -5534,7 +5534,7 @@
       <c r="T28" s="69"/>
       <c r="U28" s="69"/>
       <c r="V28" s="70" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="W28" s="70"/>
       <c r="X28" s="69"/>
@@ -5542,7 +5542,7 @@
       <c r="Z28" s="70"/>
       <c r="AA28" s="69"/>
       <c r="AB28" s="69" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AC28" s="69"/>
       <c r="AD28" s="70" t="s">
@@ -5558,10 +5558,10 @@
     </row>
     <row r="29" spans="1:37" ht="13.95" customHeight="1">
       <c r="A29" s="67" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B29" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C29" s="68"/>
       <c r="D29" s="69" t="s">
@@ -5600,7 +5600,7 @@
         <v>87</v>
       </c>
       <c r="AC29" s="69" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AD29" s="70" t="s">
         <v>62</v>
@@ -5611,11 +5611,11 @@
       <c r="AF29" s="69"/>
       <c r="AG29" s="69"/>
       <c r="AH29" s="74" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AI29" s="72"/>
       <c r="AJ29" s="75" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AK29" s="65"/>
     </row>
@@ -5624,7 +5624,7 @@
         <v>82</v>
       </c>
       <c r="B30" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C30" s="68"/>
       <c r="D30" s="69" t="s">
@@ -5692,10 +5692,10 @@
     </row>
     <row r="31" spans="1:37" ht="13.95" customHeight="1">
       <c r="A31" s="67" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B31" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C31" s="68"/>
       <c r="D31" s="69" t="s">
@@ -5714,7 +5714,7 @@
         <v>82</v>
       </c>
       <c r="I31" s="69" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J31" s="71">
         <v>32651287</v>
@@ -5754,7 +5754,7 @@
         <v>73</v>
       </c>
       <c r="B32" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C32" s="68"/>
       <c r="D32" s="69" t="s">
@@ -5796,7 +5796,7 @@
       <c r="T32" s="69"/>
       <c r="U32" s="69"/>
       <c r="V32" s="70" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="W32" s="70"/>
       <c r="X32" s="69"/>
@@ -5827,7 +5827,7 @@
         <v>54</v>
       </c>
       <c r="B33" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C33" s="68" t="s">
         <v>123</v>
@@ -5889,13 +5889,13 @@
     </row>
     <row r="34" spans="1:37" ht="13.95" customHeight="1">
       <c r="A34" s="67" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="81" t="s">
+        <v>304</v>
+      </c>
+      <c r="C34" s="68" t="s">
         <v>142</v>
-      </c>
-      <c r="B34" s="81" t="s">
-        <v>305</v>
-      </c>
-      <c r="C34" s="68" t="s">
-        <v>143</v>
       </c>
       <c r="D34" s="69" t="s">
         <v>7</v>
@@ -5910,7 +5910,7 @@
         <v>11</v>
       </c>
       <c r="H34" s="70" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I34" s="69" t="s">
         <v>76</v>
@@ -5950,13 +5950,13 @@
     </row>
     <row r="35" spans="1:37" ht="13.95" customHeight="1">
       <c r="A35" s="67" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" s="81" t="s">
+        <v>303</v>
+      </c>
+      <c r="C35" s="68" t="s">
         <v>163</v>
-      </c>
-      <c r="B35" s="81" t="s">
-        <v>304</v>
-      </c>
-      <c r="C35" s="68" t="s">
-        <v>164</v>
       </c>
       <c r="D35" s="69" t="s">
         <v>7</v>
@@ -6008,7 +6008,7 @@
         <v>77</v>
       </c>
       <c r="B36" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C36" s="68"/>
       <c r="D36" s="69" t="s">
@@ -6066,10 +6066,10 @@
     </row>
     <row r="37" spans="1:37" ht="13.95" customHeight="1">
       <c r="A37" s="67" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B37" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C37" s="68"/>
       <c r="D37" s="69" t="s">
@@ -6082,7 +6082,7 @@
         <v>9</v>
       </c>
       <c r="G37" s="69" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H37" s="70"/>
       <c r="I37" s="69"/>
@@ -6119,10 +6119,10 @@
     </row>
     <row r="38" spans="1:37" ht="13.95" customHeight="1">
       <c r="A38" s="67" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B38" s="81" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C38" s="68"/>
       <c r="D38" s="69" t="s">
@@ -6173,7 +6173,7 @@
         <v>84</v>
       </c>
       <c r="B39" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C39" s="68" t="s">
         <v>88</v>
@@ -6239,13 +6239,13 @@
     </row>
     <row r="40" spans="1:37" ht="13.95" customHeight="1">
       <c r="A40" s="67" t="s">
+        <v>164</v>
+      </c>
+      <c r="B40" s="81" t="s">
+        <v>303</v>
+      </c>
+      <c r="C40" s="68" t="s">
         <v>165</v>
-      </c>
-      <c r="B40" s="81" t="s">
-        <v>304</v>
-      </c>
-      <c r="C40" s="68" t="s">
-        <v>166</v>
       </c>
       <c r="D40" s="69" t="s">
         <v>106</v>
@@ -6290,19 +6290,19 @@
       <c r="AH40" s="70"/>
       <c r="AI40" s="72"/>
       <c r="AJ40" s="73" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AK40" s="65"/>
     </row>
     <row r="41" spans="1:37" ht="13.95" customHeight="1">
       <c r="A41" s="67" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B41" s="81" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C41" s="68" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D41" s="69" t="s">
         <v>103</v>
@@ -6328,13 +6328,13 @@
       <c r="Q41" s="70"/>
       <c r="R41" s="69"/>
       <c r="S41" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="T41" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="T41" s="69" t="s">
+      <c r="U41" s="69" t="s">
         <v>160</v>
-      </c>
-      <c r="U41" s="69" t="s">
-        <v>161</v>
       </c>
       <c r="V41" s="70"/>
       <c r="W41" s="70"/>
@@ -6343,7 +6343,7 @@
       <c r="Z41" s="70"/>
       <c r="AA41" s="69"/>
       <c r="AB41" s="69" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AC41" s="69"/>
       <c r="AD41" s="70" t="s">
@@ -6364,7 +6364,7 @@
         <v>94</v>
       </c>
       <c r="B42" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C42" s="68" t="s">
         <v>96</v>
@@ -6438,10 +6438,10 @@
     </row>
     <row r="43" spans="1:37" ht="13.95" customHeight="1">
       <c r="A43" s="67" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B43" s="81" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C43" s="68"/>
       <c r="D43" s="69" t="s">
@@ -6491,10 +6491,10 @@
     </row>
     <row r="44" spans="1:37" ht="13.95" customHeight="1">
       <c r="A44" s="67" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B44" s="81" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C44" s="68"/>
       <c r="D44" s="69" t="s">
@@ -6544,10 +6544,10 @@
     </row>
     <row r="45" spans="1:37" ht="13.95" customHeight="1">
       <c r="A45" s="67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B45" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C45" s="68"/>
       <c r="D45" s="69" t="s">
@@ -6577,12 +6577,12 @@
       <c r="T45" s="69"/>
       <c r="U45" s="69"/>
       <c r="V45" s="70" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="W45" s="70"/>
       <c r="X45" s="69"/>
       <c r="Y45" s="70" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Z45" s="70"/>
       <c r="AA45" s="69"/>
@@ -6601,10 +6601,10 @@
     </row>
     <row r="46" spans="1:37" ht="13.95" customHeight="1">
       <c r="A46" s="67" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B46" s="81" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C46" s="68"/>
       <c r="D46" s="69" t="s">
@@ -6657,7 +6657,7 @@
         <v>132</v>
       </c>
       <c r="B47" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C47" s="68"/>
       <c r="D47" s="69" t="s">
@@ -6708,7 +6708,7 @@
         <v>107</v>
       </c>
       <c r="B48" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C48" s="68" t="s">
         <v>108</v>
@@ -6781,7 +6781,7 @@
         <v>104</v>
       </c>
       <c r="B49" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C49" s="68" t="s">
         <v>105</v>
@@ -6835,10 +6835,10 @@
     </row>
     <row r="50" spans="1:37" ht="13.95" customHeight="1">
       <c r="A50" s="67" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B50" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C50" s="68"/>
       <c r="D50" s="69" t="s">
@@ -6889,7 +6889,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C51" s="68" t="s">
         <v>48</v>
@@ -6962,7 +6962,7 @@
         <v>47</v>
       </c>
       <c r="B52" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C52" s="68" t="s">
         <v>48</v>
@@ -7036,10 +7036,10 @@
     </row>
     <row r="53" spans="1:37" ht="13.95" customHeight="1">
       <c r="A53" s="67" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B53" s="81" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C53" s="68"/>
       <c r="D53" s="69" t="s">
@@ -7089,14 +7089,14 @@
     </row>
     <row r="54" spans="1:37" ht="13.95" customHeight="1">
       <c r="A54" s="67" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B54" s="81" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C54" s="68"/>
       <c r="D54" s="69" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E54" s="69" t="s">
         <v>49</v>
@@ -7131,7 +7131,7 @@
         <v>113</v>
       </c>
       <c r="AC54" s="69" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AD54" s="70" t="s">
         <v>58</v>
@@ -7149,7 +7149,7 @@
         <v>75</v>
       </c>
       <c r="B55" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C55" s="68" t="s">
         <v>128</v>
@@ -7214,7 +7214,7 @@
         <v>116</v>
       </c>
       <c r="B56" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C56" s="68" t="s">
         <v>117</v>
@@ -43917,19 +43917,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="51" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="51" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="C1" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="C1" s="51" t="s">
-        <v>232</v>
-      </c>
       <c r="D1" s="54" t="s">
+        <v>254</v>
+      </c>
+      <c r="E1" s="54" t="s">
         <v>255</v>
-      </c>
-      <c r="E1" s="54" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -43943,27 +43943,27 @@
         <v>9</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E2" s="53" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D3" s="53" t="s">
         <v>114</v>
       </c>
       <c r="E3" s="53" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -43971,16 +43971,16 @@
         <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D4" s="53" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -43988,13 +43988,13 @@
         <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E5" s="53" t="s">
         <v>58</v>
@@ -44005,16 +44005,16 @@
         <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D6" s="53" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -44022,13 +44022,13 @@
         <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D7" s="53" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E7" s="53" t="s">
         <v>62</v>
@@ -44039,10 +44039,10 @@
         <v>139</v>
       </c>
       <c r="B8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D8" s="53" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E8" s="53" t="s">
         <v>115</v>
@@ -44050,16 +44050,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D9" s="53" t="s">
         <v>113</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -44070,7 +44070,7 @@
         <v>90</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -44078,7 +44078,7 @@
         <v>106</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E11" s="53"/>
     </row>
@@ -44087,13 +44087,13 @@
         <v>89</v>
       </c>
       <c r="D12" s="55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E12" s="53"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="52" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D13" s="53" t="s">
         <v>61</v>
@@ -44102,28 +44102,28 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="52" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E14" s="53"/>
     </row>
     <row r="15" spans="1:5">
       <c r="D15" s="53" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E15" s="53"/>
     </row>
     <row r="16" spans="1:5">
       <c r="D16" s="53" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E16" s="53"/>
     </row>
     <row r="17" spans="4:5">
       <c r="D17" s="53" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E17" s="53"/>
     </row>
@@ -44141,7 +44141,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E20" s="53"/>
     </row>
@@ -44153,25 +44153,25 @@
     </row>
     <row r="22" spans="4:5">
       <c r="D22" s="53" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E22" s="53"/>
     </row>
     <row r="23" spans="4:5">
       <c r="D23" s="53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E23" s="53"/>
     </row>
     <row r="24" spans="4:5">
       <c r="D24" s="53" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E24" s="53"/>
     </row>
     <row r="25" spans="4:5">
       <c r="D25" s="53" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E25" s="53"/>
     </row>
@@ -44201,25 +44201,25 @@
     </row>
     <row r="30" spans="4:5">
       <c r="D30" s="53" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E30" s="53"/>
     </row>
     <row r="31" spans="4:5">
       <c r="D31" s="53" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E31" s="53"/>
     </row>
     <row r="32" spans="4:5">
       <c r="D32" s="53" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E32" s="53"/>
     </row>
     <row r="33" spans="4:5">
       <c r="D33" s="53" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E33" s="53"/>
     </row>
@@ -44231,37 +44231,37 @@
     </row>
     <row r="35" spans="4:5">
       <c r="D35" s="53" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E35" s="53"/>
     </row>
     <row r="36" spans="4:5">
       <c r="D36" s="53" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E36" s="53"/>
     </row>
     <row r="37" spans="4:5">
       <c r="D37" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E37" s="53"/>
     </row>
     <row r="38" spans="4:5">
       <c r="D38" s="53" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E38" s="53"/>
     </row>
     <row r="39" spans="4:5">
       <c r="D39" s="53" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E39" s="53"/>
     </row>
     <row r="40" spans="4:5">
       <c r="D40" s="53" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E40" s="53"/>
     </row>
@@ -44273,19 +44273,19 @@
     </row>
     <row r="42" spans="4:5">
       <c r="D42" s="53" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E42" s="53"/>
     </row>
     <row r="43" spans="4:5">
       <c r="D43" s="55" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E43" s="53"/>
     </row>
     <row r="44" spans="4:5">
       <c r="D44" s="55" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E44" s="53"/>
     </row>
@@ -44297,13 +44297,13 @@
     </row>
     <row r="46" spans="4:5">
       <c r="D46" s="55" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E46" s="53"/>
     </row>
     <row r="47" spans="4:5">
       <c r="D47" s="53" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E47" s="53"/>
     </row>
@@ -44321,7 +44321,7 @@
     </row>
     <row r="50" spans="4:5">
       <c r="D50" s="53" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E50" s="53"/>
     </row>
@@ -44451,31 +44451,31 @@
         <v>6</v>
       </c>
       <c r="B1" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="E1" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="F1" s="37" t="s">
         <v>214</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C2" s="37">
         <v>330</v>
       </c>
       <c r="D2" s="49"/>
       <c r="F2" s="37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
@@ -44502,7 +44502,7 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="37" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D7" s="48">
         <v>976602</v>
@@ -44513,7 +44513,7 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D8" s="49"/>
       <c r="E8" s="37">

</xml_diff>